<commit_message>
CalLab-DCC writer.xlsx is added.
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395BFC2F-8C04-4203-9336-314838D6654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3D7FFE-B410-4D85-A42D-29ED2BB59963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5335,7 +5335,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Removed DCC-template from repository
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3D7FFE-B410-4D85-A42D-29ED2BB59963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC04A0-3EBC-4243-A3BD-018CF0362D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="4275" windowWidth="32685" windowHeight="14520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="458">
   <si>
     <t>customerTag</t>
   </si>
@@ -450,21 +450,6 @@
     <t>swRef</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Customer ID</t>
-  </si>
-  <si>
-    <t>Product number</t>
-  </si>
-  <si>
-    <t>Serial number</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -1423,6 +1408,27 @@
   </si>
   <si>
     <t>LABORATORY</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>productNumber</t>
+  </si>
+  <si>
+    <t>serialNumber</t>
+  </si>
+  <si>
+    <t>customerId</t>
   </si>
 </sst>
 </file>
@@ -2853,18 +2859,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:I6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:J6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="11" xr3:uid="{E1F38CF0-334C-4B49-992A-E4DFCF5745A7}" name="Column1"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Customer ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="customerId"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="equipmentClass"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="description"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="swRef"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Manufacturer"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Product Name"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Product number"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Serial number"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="manufacturer"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="productName"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="productNumber"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="serialNumber"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3174,13 +3181,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3208,10 +3215,10 @@
         <v>40</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -3223,10 +3230,10 @@
         <v>36</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -3238,10 +3245,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -3253,10 +3260,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -3265,7 +3272,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -3278,10 +3285,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -3290,10 +3297,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D8" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -3302,10 +3309,10 @@
         <v>37</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D9" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -3314,10 +3321,10 @@
         <v>38</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -3326,10 +3333,10 @@
         <v>39</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -3338,10 +3345,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D12" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -3350,10 +3357,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -3362,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D14" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -3374,10 +3381,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -3386,10 +3393,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="L16" s="2"/>
     </row>
@@ -3398,10 +3405,10 @@
         <v>61</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -3409,10 +3416,10 @@
         <v>62</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D18" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -3420,74 +3427,74 @@
         <v>65</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D19" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D20" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D22" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D23" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D26" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D27" t="s">
         <v>49</v>
@@ -3495,39 +3502,39 @@
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D28" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D30" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D31" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
@@ -3535,637 +3542,637 @@
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D33" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D34" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D35" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D36" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D37" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D38" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D39" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D40" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D41" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D43" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D44" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D45" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D46" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D47" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D48" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D49" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D50" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D51" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D52" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D53" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D54" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D55" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D56" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D57" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D58" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D59" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D60" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D61" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D62" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D63" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D64" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D65" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D66" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D67" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="31" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="31" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="31" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="31" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="31" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="31" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="31" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="31" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="31" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="31" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="31" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="31" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="31" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="31" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="31" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="31" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="31" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="31" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="31" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="31" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="31" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="31" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="31" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="31" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="31" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="31" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="31" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="31" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="31" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="31" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="31" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="31" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="31" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="31" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="31" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="31" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="31" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="31" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="31" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="31" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="31" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="31" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="31" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="31" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="31" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="31" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="31" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="31" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="31" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="31" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="31" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="31" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="31" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="139" spans="3:3">
@@ -4388,11 +4395,11 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4406,7 +4413,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4417,7 +4424,7 @@
         <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4428,7 +4435,7 @@
         <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4442,7 +4449,7 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4453,7 +4460,7 @@
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4464,7 +4471,7 @@
         <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4475,7 +4482,7 @@
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4489,29 +4496,29 @@
         <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D10" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4525,7 +4532,7 @@
         <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4536,7 +4543,7 @@
         <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4547,7 +4554,7 @@
         <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4558,7 +4565,7 @@
         <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4569,7 +4576,7 @@
         <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4580,7 +4587,7 @@
         <v>103</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -4588,10 +4595,10 @@
         <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -4602,7 +4609,7 @@
         <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -4613,7 +4620,7 @@
         <v>108</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -4624,7 +4631,7 @@
         <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -4635,7 +4642,7 @@
         <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -4646,7 +4653,7 @@
         <v>125</v>
       </c>
       <c r="D22" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -4657,7 +4664,7 @@
         <v>114</v>
       </c>
       <c r="D23" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -4668,12 +4675,12 @@
         <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C25" s="28"/>
     </row>
@@ -4685,7 +4692,7 @@
         <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -4696,7 +4703,7 @@
         <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -4707,7 +4714,7 @@
         <v>121</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -4718,23 +4725,23 @@
         <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C30" s="28"/>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="28" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="3:3">
@@ -4790,42 +4797,42 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -4843,30 +4850,30 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" customWidth="1"/>
-    <col min="11" max="11" width="13.81640625" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="7.26953125" customWidth="1"/>
-    <col min="14" max="14" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4874,146 +4881,146 @@
         <v>127</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="72.5">
+    <row r="2" spans="1:20" ht="75">
       <c r="A2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D2" t="s">
         <v>404</v>
       </c>
-      <c r="B2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D2" t="s">
-        <v>409</v>
-      </c>
       <c r="E2" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="F2" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="75">
+      <c r="A3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D3" t="s">
+        <v>421</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>422</v>
+      </c>
+      <c r="G3" s="34" t="s">
         <v>423</v>
-      </c>
-      <c r="F2" t="s">
-        <v>422</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="72.5">
-      <c r="A3" t="s">
-        <v>404</v>
-      </c>
-      <c r="B3" t="s">
-        <v>405</v>
-      </c>
-      <c r="D3" t="s">
-        <v>426</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>419</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>427</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45">
+      <c r="A5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C5" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45">
+      <c r="A6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" t="s">
+        <v>381</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="43.5">
-      <c r="A5" t="s">
-        <v>418</v>
-      </c>
-      <c r="B5" t="s">
-        <v>414</v>
-      </c>
-      <c r="C5" t="s">
-        <v>386</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="43.5">
-      <c r="A6" t="s">
-        <v>418</v>
-      </c>
-      <c r="B6" t="s">
-        <v>415</v>
-      </c>
-      <c r="C6" t="s">
-        <v>386</v>
-      </c>
-      <c r="E6" s="34" t="s">
+    <row r="7" spans="1:20" ht="75">
+      <c r="A7" t="s">
+        <v>413</v>
+      </c>
+      <c r="B7" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="58">
-      <c r="A7" t="s">
-        <v>418</v>
-      </c>
-      <c r="B7" t="s">
-        <v>416</v>
-      </c>
       <c r="E7" s="34" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -5028,107 +5035,117 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="C1" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>135</v>
+        <v>453</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>133</v>
+        <v>454</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10">
+        <v>455</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>368</v>
+      </c>
+      <c r="G2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H2" t="s">
+        <v>374</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>375</v>
       </c>
-      <c r="B2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C3" t="s">
+        <v>446</v>
+      </c>
+      <c r="D3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E3" t="s">
+        <v>447</v>
+      </c>
+      <c r="G3" t="s">
         <v>373</v>
       </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F2" t="s">
-        <v>378</v>
-      </c>
-      <c r="G2" t="s">
-        <v>379</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>450</v>
-      </c>
-      <c r="B3" t="s">
-        <v>451</v>
-      </c>
-      <c r="C3" t="s">
-        <v>373</v>
-      </c>
-      <c r="D3" t="s">
-        <v>452</v>
-      </c>
-      <c r="F3" t="s">
-        <v>378</v>
-      </c>
-      <c r="G3" t="s">
-        <v>453</v>
-      </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>448</v>
+      </c>
+      <c r="I3">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
-        <v>454</v>
+      <c r="J3" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -5148,12 +5165,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="25.26953125" customWidth="1"/>
-    <col min="4" max="4" width="31.7265625" customWidth="1"/>
-    <col min="5" max="5" width="22.26953125" customWidth="1"/>
-    <col min="6" max="6" width="55.26953125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5162,19 +5179,19 @@
         <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D1" t="s">
         <v>129</v>
       </c>
       <c r="E1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G1" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="H1" t="s">
         <v>53</v>
@@ -5182,22 +5199,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D5" t="s">
         <v>435</v>
       </c>
-      <c r="B5" t="s">
-        <v>443</v>
-      </c>
-      <c r="C5" t="s">
-        <v>441</v>
-      </c>
-      <c r="D5" t="s">
-        <v>440</v>
-      </c>
       <c r="E5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="F5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -5205,22 +5222,22 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C6" t="s">
+        <v>436</v>
+      </c>
+      <c r="D6" t="s">
         <v>435</v>
       </c>
-      <c r="B6" t="s">
-        <v>442</v>
-      </c>
-      <c r="C6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D6" t="s">
-        <v>440</v>
-      </c>
       <c r="E6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="F6" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -5228,100 +5245,100 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B7" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C7" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D7" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E7" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F7" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G7">
         <v>9.9</v>
       </c>
       <c r="H7" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B8" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C8" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D8" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E8" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G8">
         <v>0.99</v>
       </c>
       <c r="H8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B9" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C9" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D9" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E9" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F9" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G9">
         <v>9.9</v>
       </c>
       <c r="H9" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B10" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C10" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D10" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="E10" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="F10" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -5338,21 +5355,21 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5360,7 +5377,7 @@
         <v>51</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="H1" s="35"/>
       <c r="I1" s="35"/>
@@ -5369,26 +5386,26 @@
     </row>
     <row r="2" spans="1:14" ht="17.25" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="27" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="27" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -5461,7 +5478,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="22">
+    <row r="10" spans="1:14" ht="23.25">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -5502,10 +5519,10 @@
         <v>35</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="22">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="23.25">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
@@ -5513,34 +5530,34 @@
         <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>31</v>
@@ -5549,12 +5566,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="23.25">
       <c r="A12" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>47</v>
@@ -5587,18 +5604,18 @@
         <v>49</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="32.5">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45.75">
       <c r="A13" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>27</v>
@@ -5634,7 +5651,7 @@
         <v>70</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -5680,7 +5697,7 @@
         <v>42</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -5818,7 +5835,7 @@
         <v>42</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -5864,7 +5881,7 @@
         <v>42</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes of the day
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC04A0-3EBC-4243-A3BD-018CF0362D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2251B129-B3A2-4CC0-89C3-B54403D2F8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="4275" windowWidth="32685" windowHeight="14520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6990" yWindow="3675" windowWidth="32685" windowHeight="14520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="464">
   <si>
     <t>customerTag</t>
   </si>
@@ -1429,6 +1429,24 @@
   </si>
   <si>
     <t>customerId</t>
+  </si>
+  <si>
+    <t>itemID3</t>
+  </si>
+  <si>
+    <t>another display unit</t>
+  </si>
+  <si>
+    <t>NN15</t>
+  </si>
+  <si>
+    <t>silver edition</t>
+  </si>
+  <si>
+    <t>L45</t>
+  </si>
+  <si>
+    <t>lqmdu2498710</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1659,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1736,6 +1754,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -5035,10 +5054,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5146,6 +5165,35 @@
       </c>
       <c r="J3" t="s">
         <v>449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" t="s">
+        <v>459</v>
+      </c>
+      <c r="G4" t="s">
+        <v>373</v>
+      </c>
+      <c r="H4" t="s">
+        <v>461</v>
+      </c>
+      <c r="I4" t="s">
+        <v>462</v>
+      </c>
+      <c r="J4" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -5349,10 +5397,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5421,7 +5469,6 @@
         <v>59</v>
       </c>
       <c r="B7" s="27">
-        <f>COUNTA(A14:A1048576)</f>
         <v>5</v>
       </c>
     </row>
@@ -5881,6 +5928,515 @@
         <v>42</v>
       </c>
       <c r="N18" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="27">
+        <f>COUNTA(B29:XFD29)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="23.25">
+      <c r="A30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="23.25">
+      <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="23.25">
+      <c r="A32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="45.75">
+      <c r="A33" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K33" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L33" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="18">
+        <v>0</v>
+      </c>
+      <c r="D34" s="19">
+        <f>ROUND(E34+273.15,2)</f>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E34" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="F34" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="G34" s="9">
+        <f>ROUND(F34-E34,1)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="H34" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I34" s="26">
+        <v>2</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="8">
+        <v>1</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="18">
+        <v>15</v>
+      </c>
+      <c r="D35" s="19">
+        <f t="shared" ref="D35:D38" si="2">ROUND(E35+273.15,2)</f>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E35" s="19">
+        <v>15.01</v>
+      </c>
+      <c r="F35" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" ref="G35:G38" si="3">ROUND(F35-E35,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H35" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I35" s="26">
+        <v>2</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L35" s="8">
+        <v>2</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N35" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="18">
+        <v>25</v>
+      </c>
+      <c r="D36" s="19">
+        <f t="shared" si="2"/>
+        <v>298.17</v>
+      </c>
+      <c r="E36" s="19">
+        <v>25.02</v>
+      </c>
+      <c r="F36" s="9">
+        <v>25.2</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="H36" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I36" s="26">
+        <v>2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L36" s="8">
+        <v>3</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="18">
+        <v>15</v>
+      </c>
+      <c r="D37" s="19">
+        <f t="shared" si="2"/>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E37" s="19">
+        <v>15.01</v>
+      </c>
+      <c r="F37" s="9">
+        <v>15.3</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="26">
+        <v>2</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L37" s="8">
+        <v>4</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N37" s="9" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="21">
+        <v>0</v>
+      </c>
+      <c r="D38" s="19">
+        <f t="shared" si="2"/>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E38" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I38" s="26">
+        <v>2</v>
+      </c>
+      <c r="J38" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L38" s="4">
+        <v>5</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" s="7" t="s">
         <v>410</v>
       </c>
     </row>
@@ -5891,13 +6447,13 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:N11" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:N11 B31:N31" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>MeasurandType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:N9" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:N9 B29:N29" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:N10" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:N10 B30:N30" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>MetaType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix unique table attributes
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2251B129-B3A2-4CC0-89C3-B54403D2F8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE0D7C2-D9DD-4E84-8578-A08F1025BDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="3675" windowWidth="32685" windowHeight="14520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7920" yWindow="6915" windowWidth="24315" windowHeight="11745" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="466">
   <si>
     <t>customerTag</t>
   </si>
@@ -1447,6 +1447,12 @@
   </si>
   <si>
     <t>lqmdu2498710</t>
+  </si>
+  <si>
+    <t>method01</t>
+  </si>
+  <si>
+    <t>itemID1 itemID3</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1665,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1754,7 +1760,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -4411,7 +4416,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4869,7 +4874,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5037,6 +5042,9 @@
       </c>
       <c r="B7" t="s">
         <v>411</v>
+      </c>
+      <c r="C7" t="s">
+        <v>464</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>412</v>
@@ -5399,7 +5407,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -5935,11 +5943,11 @@
       <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="27" t="s">
@@ -5954,7 +5962,7 @@
         <v>396</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>395</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:14">

</xml_diff>

<commit_message>
Update handling of statements
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -8,35 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A564B601-FF04-45B3-A772-417E753CC853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E476A6-A7E0-414F-8F0B-B0D0DB5B66BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="690" windowWidth="34320" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="690" windowWidth="34320" windowHeight="19680" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
     <sheet name="AdministrativeData" sheetId="4" r:id="rId2"/>
     <sheet name="Software" sheetId="8" r:id="rId3"/>
-    <sheet name="NewStatemens" sheetId="10" r:id="rId4"/>
-    <sheet name="Statements" sheetId="6" r:id="rId5"/>
-    <sheet name="Items" sheetId="7" r:id="rId6"/>
-    <sheet name="Equipment" sheetId="12" r:id="rId7"/>
-    <sheet name="Locations" sheetId="13" r:id="rId8"/>
-    <sheet name="Settings" sheetId="9" r:id="rId9"/>
-    <sheet name="Accreditation" sheetId="11" r:id="rId10"/>
-    <sheet name="Table2" sheetId="5" r:id="rId11"/>
+    <sheet name="Statements" sheetId="10" r:id="rId4"/>
+    <sheet name="Items" sheetId="7" r:id="rId5"/>
+    <sheet name="Settings" sheetId="9" r:id="rId6"/>
+    <sheet name="Accreditation" sheetId="11" r:id="rId7"/>
+    <sheet name="Table2" sheetId="5" r:id="rId8"/>
+    <sheet name="Locations" sheetId="13" r:id="rId9"/>
+    <sheet name="OldStatements" sheetId="6" r:id="rId10"/>
+    <sheet name="Equipment" sheetId="12" r:id="rId11"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
-    <definedName name="ColType" localSheetId="8">[1]Definitions!$A$2:$A$6</definedName>
+    <definedName name="ColType" localSheetId="5">[1]Definitions!$A$2:$A$6</definedName>
     <definedName name="ColType">Definitions!$A$2:$A$6</definedName>
     <definedName name="EquipmentCategories">Definitions!$G$2:$G$3</definedName>
-    <definedName name="MeasurandType" localSheetId="8">[1]Definitions!$C$2:$C$152</definedName>
+    <definedName name="MeasurandType" localSheetId="5">[1]Definitions!$C$2:$C$152</definedName>
     <definedName name="MeasurandType">Definitions!$C$2:$C$152</definedName>
     <definedName name="metaDataType">Definitions!$I$2:$I$11</definedName>
-    <definedName name="MetaType" localSheetId="8">[1]Definitions!$B$2:$B$21</definedName>
+    <definedName name="MetaType" localSheetId="5">[1]Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType">Definitions!$B$2:$B$21</definedName>
     <definedName name="rgKommentar">[2]ODBC!$O$7:$P$19</definedName>
     <definedName name="statementCategories">Definitions!$F$2:$F$8</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="532">
   <si>
     <t>customerTag</t>
   </si>
@@ -1463,9 +1463,6 @@
     <t>text lang1</t>
   </si>
   <si>
-    <t>description lang2</t>
-  </si>
-  <si>
     <t>Statement categories</t>
   </si>
   <si>
@@ -1484,15 +1481,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Accreditation</t>
-  </si>
-  <si>
-    <t>Heading lang1</t>
-  </si>
-  <si>
-    <t>Heading lang2</t>
-  </si>
-  <si>
     <t>Equipment Categories</t>
   </si>
   <si>
@@ -1544,9 +1532,6 @@
     <t>Name2</t>
   </si>
   <si>
-    <t>Street</t>
-  </si>
-  <si>
     <t>PostCode</t>
   </si>
   <si>
@@ -1584,6 +1569,97 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>text lang2</t>
+  </si>
+  <si>
+    <t>Dette certifikat er i overensstemmelse med måleevnerne angivet i MRA’ens Appendiks C, som er redigeret af CIPM. I henhold til MRA’en anerkender alle deltagende institutter gyldigheden af hinandens kalibrerings- og målecertifikater for de målestørrelser, måleområder og måleusikkerheder som er specificeret i Appendiks C 
+(for detaljer se www.bipm.org).</t>
+  </si>
+  <si>
+    <t>This certificate is consistent with the capabilities that are included in Appendix C of the MRA drawn up by the CIPM. Under the MRA, all participating institutes recognize the validity of each other’s calibration and measurement certificates for the quantities, ranges and measurement uncertainties specified in Appendix C (for details see http://www.bipm.org).</t>
+  </si>
+  <si>
+    <t>CIPM MRA</t>
+  </si>
+  <si>
+    <t>stabilaser</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>cust</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>kogle alle</t>
+  </si>
+  <si>
+    <t>Street1</t>
+  </si>
+  <si>
+    <t>16, 1. tv</t>
+  </si>
+  <si>
+    <t>DFM</t>
+  </si>
+  <si>
+    <t>Danish Professional Company</t>
+  </si>
+  <si>
+    <t>meth01</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Metode</t>
+  </si>
+  <si>
+    <t>heading lang1</t>
+  </si>
+  <si>
+    <t>heading lang2</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Reference Used</t>
+  </si>
+  <si>
+    <t>accreditation</t>
+  </si>
+  <si>
+    <t>accreditationLabId</t>
+  </si>
+  <si>
+    <t>accreditationBody</t>
+  </si>
+  <si>
+    <t>accreditationCountry</t>
+  </si>
+  <si>
+    <t>accreditationNorm</t>
+  </si>
+  <si>
+    <t>accreditationApplicability</t>
+  </si>
+  <si>
+    <t>accreditationException</t>
+  </si>
+  <si>
+    <t>accreditationStatement lang1</t>
   </si>
 </sst>
 </file>
@@ -1593,7 +1669,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1654,6 +1730,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1802,7 +1884,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1899,6 +1981,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3050,21 +3136,61 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCFE7457-6089-422F-AE8B-F93B5CC6D5E3}" name="Table135" displayName="Table135" ref="A1:F8" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCFE7457-6089-422F-AE8B-F93B5CC6D5E3}" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="C1:G8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B6460555-0E0D-4889-8643-C5F57DB2E042}" name="id"/>
-    <tableColumn id="7" xr3:uid="{DBA00E02-303F-43CE-90B3-51B0B1B791BA}" name="Category"/>
-    <tableColumn id="3" xr3:uid="{C1C3BF6A-959C-4D7D-AC99-517770D89042}" name="Heading lang1"/>
+    <tableColumn id="3" xr3:uid="{C1C3BF6A-959C-4D7D-AC99-517770D89042}" name="heading lang1"/>
     <tableColumn id="4" xr3:uid="{82EC8405-575B-45C9-97A5-B2BE0DFA2511}" name="text lang1" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{19BCF9E6-A96F-4617-BFC8-5BA713CC7CF5}" name="Heading lang2"/>
-    <tableColumn id="6" xr3:uid="{EC9151B2-0AB3-48BB-A419-43898218651D}" name="description lang2"/>
+    <tableColumn id="5" xr3:uid="{19BCF9E6-A96F-4617-BFC8-5BA713CC7CF5}" name="heading lang2"/>
+    <tableColumn id="6" xr3:uid="{EC9151B2-0AB3-48BB-A419-43898218651D}" name="text lang2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:J6" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="11" xr3:uid="{E1F38CF0-334C-4B49-992A-E4DFCF5745A7}" name="Column1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="customerId"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="equipmentClass"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="description"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="swRef"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="manufacturer"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="productName"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="productNumber"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="serialNumber"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1BBFECBA-56D4-4850-A69E-DDD8D8846A58}" name="Table167" displayName="Table167" ref="A1:M6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:M6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="11" xr3:uid="{04D47612-4EBB-4C61-8AA2-577AC8EF81C5}" name="Category"/>
+    <tableColumn id="1" xr3:uid="{1806EC44-C85B-49CD-AF40-4809015F8B91}" name="id"/>
+    <tableColumn id="10" xr3:uid="{037FC876-FCB0-4BD8-B949-CCDFEF3DB5C3}" name="Name1"/>
+    <tableColumn id="13" xr3:uid="{059EB501-42EB-481D-BD96-60B1F9F8E0BF}" name="Name2"/>
+    <tableColumn id="2" xr3:uid="{4B415654-8F7A-40C8-BE3F-C07A4342B8A8}" name="Street1"/>
+    <tableColumn id="3" xr3:uid="{8C44E7BB-FF2E-44D7-8032-0F3A17D4F953}" name="StreetNo"/>
+    <tableColumn id="14" xr3:uid="{D59D5E06-76EA-4FBE-A02E-AB131783E17F}" name="Column1"/>
+    <tableColumn id="4" xr3:uid="{A708A527-4B82-4729-94A7-E36DC2AB792E}" name="City"/>
+    <tableColumn id="5" xr3:uid="{F5A5DD0D-3003-45A9-975B-5FFE69D70DD2}" name="PostCode"/>
+    <tableColumn id="6" xr3:uid="{907E8258-546A-4ED6-80F0-FF4C0BB84D88}" name="PO-BOX"/>
+    <tableColumn id="7" xr3:uid="{18EA1B9E-9FA2-4BB9-B5B5-C58EAD2FEB62}" name="CountryCode"/>
+    <tableColumn id="8" xr3:uid="{BD63A030-E943-4AE2-BD22-F3A03E64E7FD}" name="further"/>
+    <tableColumn id="9" xr3:uid="{7E706009-4E8A-4143-8D41-18D74C7EFA47}" name="p"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="B1:S8" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B1:S8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
@@ -3091,28 +3217,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:J6" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{E1F38CF0-334C-4B49-992A-E4DFCF5745A7}" name="Column1"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="customerId"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="equipmentClass"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="description"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="swRef"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="manufacturer"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="productName"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="productNumber"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="serialNumber"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B838957E-BA60-4601-B76A-05754E31F1D4}" name="Table16" displayName="Table16" ref="A1:J6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B838957E-BA60-4601-B76A-05754E31F1D4}" name="Table16" displayName="Table16" ref="B1:K6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B1:K6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="11" xr3:uid="{2F03DDC1-5525-47DB-9C7A-78876A716A29}" name="Category"/>
     <tableColumn id="1" xr3:uid="{EA082D58-1E08-4AD3-BFAF-E947B2336921}" name="id"/>
@@ -3124,27 +3231,6 @@
     <tableColumn id="7" xr3:uid="{62A0306E-96DA-4535-9CFB-48AF217F6E8E}" name="productName"/>
     <tableColumn id="8" xr3:uid="{B1BA2124-70A6-4015-9AF1-FE74E51C0115}" name="productNumber"/>
     <tableColumn id="9" xr3:uid="{B433F7BB-298D-4183-A3D7-5EC8642DEF72}" name="serialNumber"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1BBFECBA-56D4-4850-A69E-DDD8D8846A58}" name="Table167" displayName="Table167" ref="A1:L6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:L6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="12">
-    <tableColumn id="11" xr3:uid="{04D47612-4EBB-4C61-8AA2-577AC8EF81C5}" name="Category"/>
-    <tableColumn id="1" xr3:uid="{1806EC44-C85B-49CD-AF40-4809015F8B91}" name="id"/>
-    <tableColumn id="10" xr3:uid="{037FC876-FCB0-4BD8-B949-CCDFEF3DB5C3}" name="Name1"/>
-    <tableColumn id="13" xr3:uid="{059EB501-42EB-481D-BD96-60B1F9F8E0BF}" name="Name2"/>
-    <tableColumn id="2" xr3:uid="{4B415654-8F7A-40C8-BE3F-C07A4342B8A8}" name="Street"/>
-    <tableColumn id="3" xr3:uid="{8C44E7BB-FF2E-44D7-8032-0F3A17D4F953}" name="StreetNo"/>
-    <tableColumn id="4" xr3:uid="{A708A527-4B82-4729-94A7-E36DC2AB792E}" name="City"/>
-    <tableColumn id="5" xr3:uid="{F5A5DD0D-3003-45A9-975B-5FFE69D70DD2}" name="PostCode"/>
-    <tableColumn id="6" xr3:uid="{907E8258-546A-4ED6-80F0-FF4C0BB84D88}" name="PO-BOX"/>
-    <tableColumn id="7" xr3:uid="{18EA1B9E-9FA2-4BB9-B5B5-C58EAD2FEB62}" name="CountryCode"/>
-    <tableColumn id="8" xr3:uid="{BD63A030-E943-4AE2-BD22-F3A03E64E7FD}" name="further"/>
-    <tableColumn id="9" xr3:uid="{7E706009-4E8A-4143-8D41-18D74C7EFA47}" name="p"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3450,7 +3536,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -3483,36 +3569,36 @@
         <v>127</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="B2" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D2" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="F2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="I2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -3533,7 +3619,7 @@
         <v>132</v>
       </c>
       <c r="G3" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
@@ -3554,7 +3640,7 @@
         <v>304</v>
       </c>
       <c r="F4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I4" t="s">
         <v>37</v>
@@ -3593,7 +3679,7 @@
         <v>306</v>
       </c>
       <c r="F6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3612,7 +3698,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>
@@ -3630,7 +3716,7 @@
         <v>307</v>
       </c>
       <c r="F8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I8" t="s">
         <v>34</v>
@@ -3648,7 +3734,7 @@
         <v>308</v>
       </c>
       <c r="I9" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -3678,7 +3764,7 @@
         <v>310</v>
       </c>
       <c r="I11" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -4574,27 +4660,27 @@
     </row>
     <row r="157" spans="3:3">
       <c r="C157" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="158" spans="3:3">
       <c r="C158" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="159" spans="3:3">
       <c r="C159" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="160" spans="3:3">
       <c r="C160" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="161" spans="3:3">
       <c r="C161" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -4739,1247 +4825,395 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D53FE5-FD05-490B-BD2B-60774A285524}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>473</v>
+    <row r="1" spans="1:20">
+      <c r="B1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="75">
+      <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2" t="s">
+        <v>414</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="75">
+      <c r="A3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B3" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" t="s">
+        <v>418</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45">
+      <c r="A5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45">
+      <c r="A6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" t="s">
+        <v>378</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="75">
+      <c r="A7" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" t="s">
+        <v>461</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="H8" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:O40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC584196-9739-4B08-B7A7-EF0413D9DC9F}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>447</v>
-      </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-    </row>
-    <row r="2" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>395</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="26">
-        <f>COUNTA(B9:XFD9)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="23.25">
-      <c r="A10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="23.25">
-      <c r="A11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="23.25">
-      <c r="A12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>502</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>502</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>502</v>
-      </c>
-      <c r="O12" s="14" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="23.25">
-      <c r="A13" s="35" t="s">
-        <v>499</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="L13" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="M13" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="34" t="s">
-        <v>404</v>
-      </c>
-      <c r="O13" s="34" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="45.75">
-      <c r="A14" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="N14" s="22" t="s">
-        <v>405</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="17">
-        <v>0</v>
-      </c>
-      <c r="D15" s="18">
-        <f>ROUND(E15+273.15,2)</f>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E15" s="18">
-        <v>0.01</v>
-      </c>
-      <c r="F15" s="9">
-        <v>-0.1</v>
-      </c>
-      <c r="G15" s="9">
-        <f>ROUND(F15-E15,1)</f>
-        <v>-0.1</v>
-      </c>
-      <c r="H15" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I15" s="25">
-        <v>2</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L15" s="8">
+    <row r="1" spans="1:12">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
+        <v>365</v>
+      </c>
+      <c r="H2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I2" t="s">
+        <v>371</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3" t="s">
+        <v>443</v>
+      </c>
+      <c r="E3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F3" t="s">
+        <v>444</v>
+      </c>
+      <c r="H3" t="s">
+        <v>370</v>
+      </c>
+      <c r="I3" t="s">
+        <v>445</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>507</v>
+      </c>
+      <c r="B4" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D4" t="s">
+        <v>457</v>
+      </c>
+      <c r="E4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F4" t="s">
+        <v>456</v>
+      </c>
+      <c r="H4" t="s">
+        <v>370</v>
+      </c>
+      <c r="I4" t="s">
+        <v>458</v>
+      </c>
+      <c r="J4" t="s">
+        <v>459</v>
+      </c>
+      <c r="K4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C5" t="s">
+        <v>475</v>
+      </c>
+      <c r="D5" t="s">
+        <v>476</v>
+      </c>
+      <c r="F5" t="s">
+        <v>478</v>
+      </c>
+      <c r="H5" t="s">
+        <v>477</v>
+      </c>
+      <c r="I5" t="s">
+        <v>506</v>
+      </c>
+      <c r="J5" t="s">
+        <v>479</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="M15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="17">
-        <v>15</v>
-      </c>
-      <c r="D16" s="18">
-        <f t="shared" ref="D16:D19" si="0">ROUND(E16+273.15,2)</f>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E16" s="18">
-        <v>15.01</v>
-      </c>
-      <c r="F16" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" ref="G16:G19" si="1">ROUND(F16-E16,1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H16" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I16" s="25">
-        <v>2</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L16" s="8">
-        <v>2</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="17">
-        <v>25</v>
-      </c>
-      <c r="D17" s="18">
-        <f t="shared" si="0"/>
-        <v>298.17</v>
-      </c>
-      <c r="E17" s="18">
-        <v>25.02</v>
-      </c>
-      <c r="F17" s="9">
-        <v>25.2</v>
-      </c>
-      <c r="G17" s="9">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="H17" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I17" s="25">
-        <v>2</v>
-      </c>
-      <c r="J17" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L17" s="8">
-        <v>3</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="17">
-        <v>15</v>
-      </c>
-      <c r="D18" s="18">
-        <f t="shared" si="0"/>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E18" s="18">
-        <v>15.01</v>
-      </c>
-      <c r="F18" s="9">
-        <v>15.3</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
-      </c>
-      <c r="H18" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I18" s="25">
-        <v>2</v>
-      </c>
-      <c r="J18" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L18" s="8">
-        <v>4</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>406</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="20">
-        <v>0</v>
-      </c>
-      <c r="D19" s="18">
-        <f t="shared" si="0"/>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E19" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I19" s="25">
-        <v>2</v>
-      </c>
-      <c r="J19" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L19" s="4">
-        <v>5</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="26" t="s">
-        <v>395</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="26">
-        <f>COUNTA(B30:XFD30)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="N30" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="O30" s="11" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="23.25">
-      <c r="A31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="N31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="O31" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="23.25">
-      <c r="A32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="M32" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="N32" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="O32" s="11" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="23.25">
-      <c r="A33" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>502</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="M33" s="14" t="s">
-        <v>502</v>
-      </c>
-      <c r="N33" s="14" t="s">
-        <v>502</v>
-      </c>
-      <c r="O33" s="14" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="23.25">
-      <c r="A34" s="35" t="s">
-        <v>499</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="J34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="K34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="L34" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="M34" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="N34" s="34" t="s">
-        <v>404</v>
-      </c>
-      <c r="O34" s="34" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="45.75">
-      <c r="A35" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L35" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="N35" s="22" t="s">
-        <v>405</v>
-      </c>
-      <c r="O35" s="22" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="17">
-        <v>0</v>
-      </c>
-      <c r="D36" s="18">
-        <f>ROUND(E36+273.15,2)</f>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E36" s="18">
-        <v>0.01</v>
-      </c>
-      <c r="F36" s="9">
-        <v>-0.1</v>
-      </c>
-      <c r="G36" s="9">
-        <f>ROUND(F36-E36,1)</f>
-        <v>-0.1</v>
-      </c>
-      <c r="H36" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I36" s="25">
-        <v>2</v>
-      </c>
-      <c r="J36" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L36" s="8">
-        <v>1</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="17">
-        <v>15</v>
-      </c>
-      <c r="D37" s="18">
-        <f t="shared" ref="D37:D40" si="2">ROUND(E37+273.15,2)</f>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E37" s="18">
-        <v>15.01</v>
-      </c>
-      <c r="F37" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G37" s="9">
-        <f t="shared" ref="G37:G40" si="3">ROUND(F37-E37,1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H37" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I37" s="25">
-        <v>2</v>
-      </c>
-      <c r="J37" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L37" s="8">
-        <v>2</v>
-      </c>
-      <c r="M37" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N37" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="O37" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="17">
-        <v>25</v>
-      </c>
-      <c r="D38" s="18">
-        <f t="shared" si="2"/>
-        <v>298.17</v>
-      </c>
-      <c r="E38" s="18">
-        <v>25.02</v>
-      </c>
-      <c r="F38" s="9">
-        <v>25.2</v>
-      </c>
-      <c r="G38" s="9">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="H38" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I38" s="25">
-        <v>2</v>
-      </c>
-      <c r="J38" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L38" s="8">
-        <v>3</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="17">
-        <v>15</v>
-      </c>
-      <c r="D39" s="18">
-        <f t="shared" si="2"/>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E39" s="18">
-        <v>15.01</v>
-      </c>
-      <c r="F39" s="9">
-        <v>15.3</v>
-      </c>
-      <c r="G39" s="9">
-        <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="H39" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I39" s="25">
-        <v>2</v>
-      </c>
-      <c r="J39" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L39" s="8">
-        <v>4</v>
-      </c>
-      <c r="M39" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N39" s="9" t="s">
-        <v>406</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="20">
-        <v>0</v>
-      </c>
-      <c r="D40" s="18">
-        <f t="shared" si="2"/>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E40" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="F40" s="7">
-        <v>0</v>
-      </c>
-      <c r="G40" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I40" s="25">
-        <v>2</v>
-      </c>
-      <c r="J40" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L40" s="4">
-        <v>5</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="O40" s="7" t="s">
-        <v>505</v>
-      </c>
     </row>
   </sheetData>
-  <dataConsolidate/>
-  <mergeCells count="1">
-    <mergeCell ref="G1:K1"/>
-  </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:O11 B32:O32" xr:uid="{00000000-0002-0000-0500-000000000000}">
-      <formula1>MeasurandType</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:O9 B30:O30" xr:uid="{00000000-0002-0000-0500-000001000000}">
-      <formula1>ColType</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:O10 B31:O31" xr:uid="{00000000-0002-0000-0500-000002000000}">
-      <formula1>MetaType</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:O13 B34:O34" xr:uid="{FB1CB67C-7785-4D42-8012-3FA40F22C35C}">
-      <formula1>metaDataType</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{948C0099-BC74-4A90-BEFC-CB4A50D83A3C}">
+      <formula1>EquipmentCategories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5989,7 +5223,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6443,129 +5677,158 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EB6A2-D607-49A1-9D65-9E8022B0E74E}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" style="33" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="B1" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>465</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>475</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="75">
+        <v>521</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="75">
       <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2" t="s">
+        <v>519</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75">
+      <c r="A3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B3" t="s">
+        <v>467</v>
+      </c>
+      <c r="C3" t="s">
         <v>378</v>
       </c>
-      <c r="B2" t="s">
-        <v>468</v>
-      </c>
-      <c r="C2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>415</v>
-      </c>
-      <c r="E2" t="s">
-        <v>414</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="75">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>418</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="111.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" t="s">
         <v>397</v>
       </c>
-      <c r="B3" t="s">
-        <v>468</v>
-      </c>
-      <c r="C3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>411</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>398</v>
-      </c>
-      <c r="B4" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45">
+      <c r="D4" t="s">
+        <v>505</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>504</v>
+      </c>
+      <c r="F4" t="s">
+        <v>505</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="B5" t="s">
         <v>410</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="C5" t="s">
+        <v>406</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" t="s">
         <v>407</v>
       </c>
-      <c r="B6" t="s">
-        <v>410</v>
-      </c>
-      <c r="D6" s="33" t="s">
+      <c r="E6" s="33" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75">
+    <row r="7" spans="1:8" ht="75">
       <c r="A7" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="B7" t="s">
         <v>410</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="C7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E7" s="33" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="B8" t="s">
-        <v>468</v>
-      </c>
+    <row r="8" spans="1:8">
+      <c r="B8" s="37"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -6583,202 +5846,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:T8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20">
-      <c r="B1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" ht="75">
-      <c r="A2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>415</v>
-      </c>
-      <c r="F2" t="s">
-        <v>414</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="75">
-      <c r="A3" t="s">
-        <v>396</v>
-      </c>
-      <c r="B3" t="s">
-        <v>397</v>
-      </c>
-      <c r="D3" t="s">
-        <v>418</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>411</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>396</v>
-      </c>
-      <c r="B4" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="45">
-      <c r="A5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B5" t="s">
-        <v>406</v>
-      </c>
-      <c r="C5" t="s">
-        <v>378</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="45">
-      <c r="A6" t="s">
-        <v>410</v>
-      </c>
-      <c r="B6" t="s">
-        <v>407</v>
-      </c>
-      <c r="C6" t="s">
-        <v>378</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="75">
-      <c r="A7" t="s">
-        <v>410</v>
-      </c>
-      <c r="B7" t="s">
-        <v>408</v>
-      </c>
-      <c r="C7" t="s">
-        <v>461</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="H8" t="s">
-        <v>463</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K4"/>
@@ -6931,380 +5998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC584196-9739-4B08-B7A7-EF0413D9DC9F}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D2" t="s">
-        <v>365</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G2" t="s">
-        <v>370</v>
-      </c>
-      <c r="H2" t="s">
-        <v>371</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>449</v>
-      </c>
-      <c r="B3" t="s">
-        <v>442</v>
-      </c>
-      <c r="C3" t="s">
-        <v>443</v>
-      </c>
-      <c r="D3" t="s">
-        <v>365</v>
-      </c>
-      <c r="E3" t="s">
-        <v>444</v>
-      </c>
-      <c r="G3" t="s">
-        <v>370</v>
-      </c>
-      <c r="H3" t="s">
-        <v>445</v>
-      </c>
-      <c r="I3">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>449</v>
-      </c>
-      <c r="B4" t="s">
-        <v>455</v>
-      </c>
-      <c r="C4" t="s">
-        <v>457</v>
-      </c>
-      <c r="D4" t="s">
-        <v>365</v>
-      </c>
-      <c r="E4" t="s">
-        <v>456</v>
-      </c>
-      <c r="G4" t="s">
-        <v>370</v>
-      </c>
-      <c r="H4" t="s">
-        <v>458</v>
-      </c>
-      <c r="I4" t="s">
-        <v>459</v>
-      </c>
-      <c r="J4" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>478</v>
-      </c>
-      <c r="B5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C5" t="s">
-        <v>480</v>
-      </c>
-      <c r="E5" t="s">
-        <v>482</v>
-      </c>
-      <c r="G5" t="s">
-        <v>481</v>
-      </c>
-      <c r="H5" t="s">
-        <v>458</v>
-      </c>
-      <c r="I5" t="s">
-        <v>483</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{948C0099-BC74-4A90-BEFC-CB4A50D83A3C}">
-      <formula1>EquipmentCategories</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6D6EC4-A3DC-42B4-ABAF-F3EE7418B168}">
-  <dimension ref="A1:M5"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E2" t="s">
-        <v>369</v>
-      </c>
-      <c r="F2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" t="s">
-        <v>365</v>
-      </c>
-      <c r="I2" t="s">
-        <v>370</v>
-      </c>
-      <c r="J2" t="s">
-        <v>371</v>
-      </c>
-      <c r="K2">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>449</v>
-      </c>
-      <c r="B3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E3" t="s">
-        <v>443</v>
-      </c>
-      <c r="F3" t="s">
-        <v>365</v>
-      </c>
-      <c r="G3" t="s">
-        <v>444</v>
-      </c>
-      <c r="I3" t="s">
-        <v>370</v>
-      </c>
-      <c r="J3" t="s">
-        <v>445</v>
-      </c>
-      <c r="K3">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>449</v>
-      </c>
-      <c r="B4" t="s">
-        <v>455</v>
-      </c>
-      <c r="E4" t="s">
-        <v>457</v>
-      </c>
-      <c r="F4" t="s">
-        <v>365</v>
-      </c>
-      <c r="G4" t="s">
-        <v>456</v>
-      </c>
-      <c r="I4" t="s">
-        <v>370</v>
-      </c>
-      <c r="J4" t="s">
-        <v>458</v>
-      </c>
-      <c r="K4" t="s">
-        <v>459</v>
-      </c>
-      <c r="L4" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>478</v>
-      </c>
-      <c r="B5" t="s">
-        <v>479</v>
-      </c>
-      <c r="E5" t="s">
-        <v>480</v>
-      </c>
-      <c r="G5" t="s">
-        <v>482</v>
-      </c>
-      <c r="I5" t="s">
-        <v>481</v>
-      </c>
-      <c r="J5" t="s">
-        <v>458</v>
-      </c>
-      <c r="K5" t="s">
-        <v>483</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{634795E6-38DB-4499-B463-CE4375BFDBB6}">
-      <formula1>EquipmentCategories</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164255F3-93CF-4992-BB4A-5F2B2030CF33}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H10"/>
@@ -7492,4 +6186,1473 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D53FE5-FD05-490B-BD2B-60774A285524}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E1" t="s">
+        <v>528</v>
+      </c>
+      <c r="F1" t="s">
+        <v>529</v>
+      </c>
+      <c r="G1" t="s">
+        <v>531</v>
+      </c>
+      <c r="I1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2">
+        <v>255</v>
+      </c>
+      <c r="E2">
+        <v>17025</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:P40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+    </row>
+    <row r="2" spans="1:16" ht="17.25" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="26">
+        <f>COUNTA(B9:XFD9)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="23.25">
+      <c r="A10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="23.25">
+      <c r="A11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="23.25">
+      <c r="A12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="23.25">
+      <c r="A13" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45.75">
+      <c r="A14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0</v>
+      </c>
+      <c r="D15" s="18">
+        <f>ROUND(E15+273.15,2)</f>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="F15" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="G15" s="9">
+        <f>ROUND(F15-E15,1)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I15" s="25">
+        <v>2</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="8">
+        <v>1</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="17">
+        <v>15</v>
+      </c>
+      <c r="D16" s="18">
+        <f t="shared" ref="D16:D19" si="0">ROUND(E16+273.15,2)</f>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E16" s="18">
+        <v>15.01</v>
+      </c>
+      <c r="F16" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" ref="G16:G19" si="1">ROUND(F16-E16,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I16" s="25">
+        <v>2</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="8">
+        <v>2</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="17">
+        <v>25</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" si="0"/>
+        <v>298.17</v>
+      </c>
+      <c r="E17" s="18">
+        <v>25.02</v>
+      </c>
+      <c r="F17" s="9">
+        <v>25.2</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="25">
+        <v>2</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="8">
+        <v>3</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="17">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18">
+        <f t="shared" si="0"/>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E18" s="18">
+        <v>15.01</v>
+      </c>
+      <c r="F18" s="9">
+        <v>15.3</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I18" s="25">
+        <v>2</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="8">
+        <v>4</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0</v>
+      </c>
+      <c r="D19" s="18">
+        <f t="shared" si="0"/>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E19" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I19" s="25">
+        <v>2</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19" s="4">
+        <v>5</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="26">
+        <f>COUNTA(B30:XFD30)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="23.25">
+      <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="23.25">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="23.25">
+      <c r="A33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="23.25">
+      <c r="A34" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="K34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="L34" s="34" t="s">
+        <v>496</v>
+      </c>
+      <c r="M34" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="O34" s="34" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="45.75">
+      <c r="A35" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="N35" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="O35" s="22" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="17">
+        <v>0</v>
+      </c>
+      <c r="D36" s="18">
+        <f>ROUND(E36+273.15,2)</f>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E36" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="F36" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="G36" s="9">
+        <f>ROUND(F36-E36,1)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="H36" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I36" s="25">
+        <v>2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L36" s="8">
+        <v>1</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N36" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="17">
+        <v>15</v>
+      </c>
+      <c r="D37" s="18">
+        <f t="shared" ref="D37:D40" si="2">ROUND(E37+273.15,2)</f>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E37" s="18">
+        <v>15.01</v>
+      </c>
+      <c r="F37" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" ref="G37:G40" si="3">ROUND(F37-E37,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="25">
+        <v>2</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L37" s="8">
+        <v>2</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N37" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="O37" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="17">
+        <v>25</v>
+      </c>
+      <c r="D38" s="18">
+        <f t="shared" si="2"/>
+        <v>298.17</v>
+      </c>
+      <c r="E38" s="18">
+        <v>25.02</v>
+      </c>
+      <c r="F38" s="9">
+        <v>25.2</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I38" s="25">
+        <v>2</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L38" s="8">
+        <v>3</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="O38" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="17">
+        <v>15</v>
+      </c>
+      <c r="D39" s="18">
+        <f t="shared" si="2"/>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E39" s="18">
+        <v>15.01</v>
+      </c>
+      <c r="F39" s="9">
+        <v>15.3</v>
+      </c>
+      <c r="G39" s="9">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="H39" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I39" s="25">
+        <v>2</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" s="8">
+        <v>4</v>
+      </c>
+      <c r="M39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N39" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="O39" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="20">
+        <v>0</v>
+      </c>
+      <c r="D40" s="18">
+        <f t="shared" si="2"/>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E40" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+      <c r="G40" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I40" s="25">
+        <v>2</v>
+      </c>
+      <c r="J40" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L40" s="4">
+        <v>5</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:P11 B32:O32" xr:uid="{00000000-0002-0000-0500-000000000000}">
+      <formula1>MeasurandType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:P9 B30:O30" xr:uid="{00000000-0002-0000-0500-000001000000}">
+      <formula1>ColType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:P10 B31:O31" xr:uid="{00000000-0002-0000-0500-000002000000}">
+      <formula1>MetaType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:P13 B34:O34" xr:uid="{FB1CB67C-7785-4D42-8012-3FA40F22C35C}">
+      <formula1>metaDataType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6D6EC4-A3DC-42B4-ABAF-F3EE7418B168}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="45">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>516</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
+        <v>514</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2">
+        <v>9218</v>
+      </c>
+      <c r="K2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C3" t="s">
+        <v>515</v>
+      </c>
+      <c r="E3" t="s">
+        <v>512</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3">
+        <v>2970</v>
+      </c>
+      <c r="K3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>511</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Allow for reading empty collumns from a DCR
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1499F98F-4FC3-4024-ADEF-AAC42FBC3BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9B512F-AE5C-49CE-BDE2-4A7E90C0F1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="690" windowWidth="34320" windowHeight="19680" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1913,7 +1913,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -2012,17 +2012,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6462,7 +6459,7 @@
     <col min="7" max="7" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7">
       <c r="B1" s="3" t="s">
         <v>516</v>
       </c>
@@ -6483,48 +6480,48 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="270" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>390</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>461</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>525</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>527</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>533</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>528</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="39" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="65.25" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>390</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="38" t="s">
         <v>526</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="39" t="s">
         <v>529</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="39" t="s">
         <v>531</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="39" t="s">
         <v>530</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="39" t="s">
         <v>532</v>
       </c>
     </row>
@@ -6543,8 +6540,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6569,13 +6566,13 @@
       <c r="A1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="40" t="s">
         <v>441</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="2" spans="1:16" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
@@ -6938,11 +6935,9 @@
       </c>
       <c r="D15" s="18">
         <f>ROUND(E15+273.15,2)</f>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E15" s="18">
-        <v>0.01</v>
-      </c>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E15" s="18"/>
       <c r="F15" s="9">
         <v>-0.1</v>
       </c>
@@ -6990,17 +6985,15 @@
       </c>
       <c r="D16" s="18">
         <f t="shared" ref="D16:D19" si="0">ROUND(E16+273.15,2)</f>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E16" s="18">
-        <v>15.01</v>
-      </c>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E16" s="18"/>
       <c r="F16" s="9">
         <v>15.1</v>
       </c>
       <c r="G16" s="9">
         <f t="shared" ref="G16:G19" si="1">ROUND(F16-E16,1)</f>
-        <v>0.1</v>
+        <v>15.1</v>
       </c>
       <c r="H16" s="24">
         <v>0.05</v>
@@ -7042,17 +7035,15 @@
       </c>
       <c r="D17" s="18">
         <f t="shared" si="0"/>
-        <v>298.17</v>
-      </c>
-      <c r="E17" s="18">
-        <v>25.02</v>
-      </c>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E17" s="18"/>
       <c r="F17" s="9">
         <v>25.2</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>25.2</v>
       </c>
       <c r="H17" s="24">
         <v>0.05</v>
@@ -7094,17 +7085,15 @@
       </c>
       <c r="D18" s="18">
         <f t="shared" si="0"/>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E18" s="18">
-        <v>15.01</v>
-      </c>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E18" s="18"/>
       <c r="F18" s="9">
         <v>15.3</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>15.3</v>
       </c>
       <c r="H18" s="24">
         <v>0.05</v>
@@ -7146,11 +7135,9 @@
       </c>
       <c r="D19" s="18">
         <f t="shared" si="0"/>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E19" s="21">
-        <v>0.01</v>
-      </c>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E19" s="21"/>
       <c r="F19" s="7">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Align accreditation statements with other statements
</commit_message>
<xml_diff>
--- a/CalLab-DCC-writer.xlsx
+++ b/CalLab-DCC-writer.xlsx
@@ -8,39 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9B512F-AE5C-49CE-BDE2-4A7E90C0F1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28893198-6A8C-4D2C-AD79-86BEB7FC7F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="690" windowWidth="34320" windowHeight="19680" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
     <sheet name="AdministrativeData" sheetId="4" r:id="rId2"/>
-    <sheet name="Software" sheetId="8" r:id="rId3"/>
-    <sheet name="Statements" sheetId="10" r:id="rId4"/>
-    <sheet name="Items" sheetId="7" r:id="rId5"/>
-    <sheet name="Settings" sheetId="9" r:id="rId6"/>
-    <sheet name="Accreditation" sheetId="11" r:id="rId7"/>
-    <sheet name="AccreditationStatements" sheetId="14" r:id="rId8"/>
-    <sheet name="Table2" sheetId="5" r:id="rId9"/>
-    <sheet name="Locations" sheetId="13" r:id="rId10"/>
-    <sheet name="OldStatements" sheetId="6" r:id="rId11"/>
-    <sheet name="Equipment" sheetId="12" r:id="rId12"/>
+    <sheet name="Statements" sheetId="10" r:id="rId3"/>
+    <sheet name="Items" sheetId="7" r:id="rId4"/>
+    <sheet name="Settings" sheetId="9" r:id="rId5"/>
+    <sheet name="Accreditation" sheetId="11" r:id="rId6"/>
+    <sheet name="Table2" sheetId="5" r:id="rId7"/>
+    <sheet name="Software" sheetId="8" r:id="rId8"/>
+    <sheet name="Locations" sheetId="13" r:id="rId9"/>
+    <sheet name="OldStatements" sheetId="6" r:id="rId10"/>
+    <sheet name="Equipment" sheetId="12" r:id="rId11"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
-    <definedName name="ColType" localSheetId="5">[1]Definitions!$A$2:$A$6</definedName>
+    <definedName name="ColType" localSheetId="4">[1]Definitions!$A$2:$A$6</definedName>
     <definedName name="ColType">Definitions!$A$2:$A$6</definedName>
     <definedName name="EquipmentCategories">Definitions!$G$2:$G$3</definedName>
-    <definedName name="MeasurandType" localSheetId="5">[1]Definitions!$C$2:$C$152</definedName>
+    <definedName name="MeasurandType" localSheetId="4">[1]Definitions!$C$2:$C$152</definedName>
     <definedName name="MeasurandType">Definitions!$C$2:$C$152</definedName>
     <definedName name="metaDataType">Definitions!$I$2:$I$11</definedName>
-    <definedName name="MetaType" localSheetId="5">[1]Definitions!$B$2:$B$21</definedName>
+    <definedName name="MetaType" localSheetId="4">[1]Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType">Definitions!$B$2:$B$21</definedName>
     <definedName name="rgKommentar">[2]ODBC!$O$7:$P$19</definedName>
-    <definedName name="statementCategories">Definitions!$F$2:$F$8</definedName>
+    <definedName name="statementCategories">Definitions!$F$2:$F$10</definedName>
     <definedName name="UsedReference">metaDataType</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="542">
   <si>
     <t>customerTag</t>
   </si>
@@ -1443,9 +1442,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>text lang1</t>
-  </si>
-  <si>
     <t>Statement categories</t>
   </si>
   <si>
@@ -1539,9 +1535,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Basis of conformity statement</t>
   </si>
   <si>
@@ -1552,9 +1545,6 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>text lang2</t>
   </si>
   <si>
     <t>Dette certifikat er i overensstemmelse med måleevnerne angivet i MRA’ens Appendiks C, som er redigeret af CIPM. I henhold til MRA’en anerkender alle deltagende institutter gyldigheden af hinandens kalibrerings- og målecertifikater for de målestørrelser, måleområder og måleusikkerheder som er specificeret i Appendiks C 
@@ -1689,6 +1679,21 @@
   </si>
   <si>
     <t>Accreditation exception</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>body lang1</t>
+  </si>
+  <si>
+    <t>body lang2</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>softwareInstruction</t>
   </si>
 </sst>
 </file>
@@ -3154,6 +3159,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCFE7457-6089-422F-AE8B-F93B5CC6D5E3}" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="C1:G8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B6460555-0E0D-4889-8643-C5F57DB2E042}" name="id"/>
+    <tableColumn id="3" xr3:uid="{C1C3BF6A-959C-4D7D-AC99-517770D89042}" name="heading lang1"/>
+    <tableColumn id="4" xr3:uid="{82EC8405-575B-45C9-97A5-B2BE0DFA2511}" name="body lang1" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{19BCF9E6-A96F-4617-BFC8-5BA713CC7CF5}" name="heading lang2"/>
+    <tableColumn id="6" xr3:uid="{EC9151B2-0AB3-48BB-A419-43898218651D}" name="body lang2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:I6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="9">
+    <tableColumn id="11" xr3:uid="{E1F38CF0-334C-4B49-992A-E4DFCF5745A7}" name="Column1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="customerId"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="description"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="swRef"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="manufacturer"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="productName"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="productNumber"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="serialNumber"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
@@ -3165,39 +3202,6 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="content"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="file"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="formula"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCFE7457-6089-422F-AE8B-F93B5CC6D5E3}" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="C1:G8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B6460555-0E0D-4889-8643-C5F57DB2E042}" name="id"/>
-    <tableColumn id="3" xr3:uid="{C1C3BF6A-959C-4D7D-AC99-517770D89042}" name="heading lang1"/>
-    <tableColumn id="4" xr3:uid="{82EC8405-575B-45C9-97A5-B2BE0DFA2511}" name="text lang1" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{19BCF9E6-A96F-4617-BFC8-5BA713CC7CF5}" name="heading lang2"/>
-    <tableColumn id="6" xr3:uid="{EC9151B2-0AB3-48BB-A419-43898218651D}" name="text lang2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:J6" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{E1F38CF0-334C-4B49-992A-E4DFCF5745A7}" name="Column1"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="customerId"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="equipmentClass"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="description"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="swRef"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="manufacturer"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="productName"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="productNumber"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="serialNumber"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3253,13 +3257,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B838957E-BA60-4601-B76A-05754E31F1D4}" name="Table16" displayName="Table16" ref="B1:K6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B1:K6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B838957E-BA60-4601-B76A-05754E31F1D4}" name="Table16" displayName="Table16" ref="B1:J6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="9">
     <tableColumn id="11" xr3:uid="{2F03DDC1-5525-47DB-9C7A-78876A716A29}" name="Category"/>
     <tableColumn id="1" xr3:uid="{EA082D58-1E08-4AD3-BFAF-E947B2336921}" name="id"/>
     <tableColumn id="2" xr3:uid="{B3FE107D-F1F8-4BA2-84D0-A4D664DA995B}" name="customerId"/>
-    <tableColumn id="3" xr3:uid="{CF41EA66-343D-4F9F-B293-63BAF024C309}" name="equipmentClass"/>
     <tableColumn id="4" xr3:uid="{257C57BA-5D0B-43F6-8D17-14F18E0B544F}" name="description"/>
     <tableColumn id="5" xr3:uid="{8AA00CC2-F293-4BB3-A2C4-3B7F057C76DC}" name="swRef"/>
     <tableColumn id="6" xr3:uid="{7A627269-42D2-425E-AC8C-45EC7EDF2E8C}" name="manufacturer"/>
@@ -3572,7 +3575,7 @@
   <dimension ref="A1:L161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3604,36 +3607,36 @@
         <v>121</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>491</v>
+        <v>537</v>
       </c>
       <c r="B2" t="s">
-        <v>491</v>
+        <v>537</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>491</v>
+        <v>537</v>
       </c>
       <c r="D2" t="s">
-        <v>491</v>
+        <v>537</v>
       </c>
       <c r="F2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -3654,10 +3657,10 @@
         <v>126</v>
       </c>
       <c r="G3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -3675,10 +3678,10 @@
         <v>298</v>
       </c>
       <c r="F4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I4" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -3699,7 +3702,7 @@
         <v>404</v>
       </c>
       <c r="I5" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -3714,7 +3717,7 @@
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3733,7 +3736,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>
@@ -3751,10 +3754,10 @@
         <v>301</v>
       </c>
       <c r="F8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I8" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -3768,8 +3771,11 @@
       <c r="D9" t="s">
         <v>302</v>
       </c>
+      <c r="F9" t="s">
+        <v>515</v>
+      </c>
       <c r="I9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -3783,6 +3789,9 @@
       <c r="D10" t="s">
         <v>303</v>
       </c>
+      <c r="F10" t="s">
+        <v>521</v>
+      </c>
       <c r="I10" t="s">
         <v>398</v>
       </c>
@@ -3799,7 +3808,7 @@
         <v>304</v>
       </c>
       <c r="I11" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -4695,314 +4704,170 @@
     </row>
     <row r="157" spans="3:3">
       <c r="C157" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="158" spans="3:3">
       <c r="C158" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="159" spans="3:3">
       <c r="C159" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="160" spans="3:3">
       <c r="C160" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="161" spans="3:3">
       <c r="C161" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-capacitance/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductance/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://www.metrology.net/wiki/testprocess-measure-conductivity/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId8" display="https://www.metrology.net/wiki/testprocess-measure-current-dc/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId9" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId11" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://www.metrology.net/wiki/testprocess-measure-force/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" display="https://www.metrology.net/wiki/testprocess-measure-frequency/" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C15" r:id="rId14" display="https://www.metrology.net/wiki/testprocess-measure-frequency-amplitudemodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C16" r:id="rId15" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-deviation/" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C17" r:id="rId16" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C18" r:id="rId17" display="https://www.metrology.net/wiki/testprocess-measure-frequency-phasemodulation-rate/" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C19" r:id="rId18" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C20" r:id="rId19" display="https://www.metrology.net/wiki/testprocess-measure-impedance/" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C21" r:id="rId20" display="https://www.metrology.net/wiki/testprocess-measure-inductance/" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C22" r:id="rId21" display="https://www.metrology.net/wiki/testprocess-measure-length/" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C23" r:id="rId22" display="https://www.metrology.net/wiki/testprocess-measure-length-circumference/" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C24" r:id="rId23" display="https://www.metrology.net/wiki/testprocess-measure-length-diameter/" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C25" r:id="rId24" display="https://www.metrology.net/wiki/testprocess-measure-length-form-flatness/" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C26" r:id="rId25" display="https://www.metrology.net/wiki/testprocess-measure-length-form-parallelism/" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C27" r:id="rId26" display="https://www.metrology.net/wiki/testprocess-measure-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C28" r:id="rId27" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roughness/" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C29" r:id="rId28" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C30" r:id="rId29" display="https://www.metrology.net/wiki/testprocess-measure-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C31" r:id="rId30" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-axis/" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C32" r:id="rId31" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-surface/" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C33" r:id="rId32" display="https://www.metrology.net/wiki/testprocess-measure-length-radius/" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C34" r:id="rId33" display="https://www.metrology.net/wiki/testprocess-measure-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C35" r:id="rId34" display="https://www.metrology.net/wiki/testprocess-measure-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C36" r:id="rId35" display="https://www.metrology.net/wiki/testprocess-measure-mass-true/" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C37" r:id="rId36" display="https://www.metrology.net/wiki/testprocess-measure-phase-phasemodulation/" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C38" r:id="rId37" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C39" r:id="rId38" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent/" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C40" r:id="rId39" display="https://www.metrology.net/wiki/testprocess-measure-phasenoise-sideband/" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C41" r:id="rId40" display="https://www.metrology.net/wiki/testprocess-measure-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C42" r:id="rId41" display="https://www.metrology.net/wiki/testprocess-measure-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C43" r:id="rId42" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C44" r:id="rId43" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C45" r:id="rId44" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C46" r:id="rId45" display="https://www.metrology.net/wiki/testprocess-measure-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C47" r:id="rId46" display="https://www.metrology.net/wiki/testprocess-measure-ratio-density-mass/" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C48" r:id="rId47" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C49" r:id="rId48" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C50" r:id="rId49" display="https://www.metrology.net/wiki/testprocess-measure-ratio-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C51" r:id="rId50" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C52" r:id="rId51" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-power/" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C53" r:id="rId52" display="https://www.metrology.net/wiki/testprocess-measure-ratio-transmissioncoefficent/" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C54" r:id="rId53" display="https://www.metrology.net/wiki/testprocess-measure-ratio-torque/" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C55" r:id="rId54" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-ripple-ondc/" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C56" r:id="rId55" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C57" r:id="rId56" display="https://www.metrology.net/wiki/testprocess-measure-ratio-volts-ac-sinewave-delta-volts/" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C58" r:id="rId57" display="https://www.metrology.net/wiki/testprocess-measure-ohms/" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C59" r:id="rId58" display="https://www.metrology.net/wiki/testprocess-measure-temperature/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C60" r:id="rId59" display="https://www.metrology.net/wiki/testprocess-measure-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C61" r:id="rId60" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C62" r:id="rId61" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C63" r:id="rId62" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C64" r:id="rId63" display="https://www.metrology.net/wiki/testprocess-measure-time-pulsetransition/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C65" r:id="rId64" display="https://www.metrology.net/wiki/testprocess-measure-time-absolute/" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C66" r:id="rId65" display="https://www.metrology.net/wiki/testprocess-measure-torque/" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C67" r:id="rId66" display="https://www.metrology.net/wiki/testprocess-measure-torque-hydraulicpressure/" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C68" r:id="rId67" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac/" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C69" r:id="rId68" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-noise-ondc/" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="C70" r:id="rId69" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="C71" r:id="rId70" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C72" r:id="rId71" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="C73" r:id="rId72" display="https://www.metrology.net/wiki/testprocess-measure-voltage-dc/" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C74" r:id="rId73" display="https://www.metrology.net/wiki/testprocess-measure-weight/" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="C75" r:id="rId74" display="https://www.metrology.net/wiki/testprocess-source-capacitance/" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C76" r:id="rId75" display="https://www.metrology.net/wiki/testprocess-source-conductance/" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C77" r:id="rId76" display="https://www.metrology.net/wiki/testprocess-source-conductivity/" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C78" r:id="rId77" display="https://www.metrology.net/wiki/testprocess-source-current-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="C79" r:id="rId78" display="https://www.metrology.net/wiki/testprocess-source-current-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C80" r:id="rId79" display="https://www.metrology.net/wiki/testprocess-source-current-ac-triangle/" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="C81" r:id="rId80" display="https://www.metrology.net/wiki/testprocess-source-current-dc/" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C82" r:id="rId81" display="https://www.metrology.net/wiki/testprocess-source-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="C83" r:id="rId82" display="https://www.metrology.net/wiki/testprocess-source-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C84" r:id="rId83" display="https://www.metrology.net/wiki/testprocess-source-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="C85" r:id="rId84" display="https://www.metrology.net/wiki/testprocess-source-force/" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="C86" r:id="rId85" display="https://www.metrology.net/wiki/testprocess-source-frequency-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C87" r:id="rId86" display="https://www.metrology.net/wiki/testprocess-source-frequency-arbitrary-cardiograph/" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C88" r:id="rId87" display="https://www.metrology.net/wiki/testprocess-source-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="C89" r:id="rId88" display="https://www.metrology.net/wiki/testprocess-source-impedance/" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C90" r:id="rId89" display="https://www.metrology.net/wiki/testprocess-source-inductance/" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C91" r:id="rId90" display="https://www.metrology.net/wiki/testprocess-source-length/" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="C92" r:id="rId91" display="https://www.metrology.net/wiki/testprocess-source-length-circumference/" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C93" r:id="rId92" display="https://www.metrology.net/wiki/testprocess-source-length-diameter/" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="C94" r:id="rId93" display="https://www.metrology.net/wiki/testprocess-source-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C95" r:id="rId94" display="https://www.metrology.net/wiki/testprocess-source-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="C96" r:id="rId95" display="https://www.metrology.net/wiki/testprocess-source-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="C97" r:id="rId96" display="https://www.metrology.net/wiki/testprocess-source-length-form-straightness-surrface/" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C98" r:id="rId97" display="https://www.metrology.net/wiki/testprocess-source-length-radius/" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="C99" r:id="rId98" display="https://www.metrology.net/wiki/testprocess-source-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="C100" r:id="rId99" display="https://www.metrology.net/wiki/testprocess-source-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C101" r:id="rId100" display="https://www.metrology.net/wiki/testprocess-source-mass-true/" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="C102" r:id="rId101" display="https://www.metrology.net/wiki/testprocess-source-period-marker/" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C103" r:id="rId102" display="https://www.metrology.net/wiki/testprocess-source-period-squarewave/" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C104" r:id="rId103" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C105" r:id="rId104" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave-simulated/" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C106" r:id="rId105" display="https://www.metrology.net/wiki/testprocess-source-power-dc-simulated/" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="C107" r:id="rId106" display="https://www.metrology.net/wiki/testprocess-source-power-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="C108" r:id="rId107" display="https://www.metrology.net/wiki/testprocess-source-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="C109" r:id="rId108" display="https://www.metrology.net/wiki/testprocess-source-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="C110" r:id="rId109" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="C111" r:id="rId110" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="C112" r:id="rId111" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C113" r:id="rId112" display="https://www.metrology.net/wiki/testprocess-source-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="C114" r:id="rId113" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="C115" r:id="rId114" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="C116" r:id="rId115" display="https://www.metrology.net/wiki/testprocess-source-ratio-rf-sinusoidal-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="C117" r:id="rId116" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="C118" r:id="rId117" display="https://www.metrology.net/wiki/testprocess-source-voltage-ac-sinewave-delta-voltage/" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="C119" r:id="rId118" display="https://www.metrology.net/wiki/testprocess-source-resistance/" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="C120" r:id="rId119" display="https://www.metrology.net/wiki/testprocess-source-temperature/" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="C121" r:id="rId120" display="https://www.metrology.net/wiki/testprocess-source-temperature-fixedpoint/" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="C122" r:id="rId121" display="https://www.metrology.net/wiki/testprocess-source-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="C123" r:id="rId122" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="C124" r:id="rId123" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="C125" r:id="rId124" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="C126" r:id="rId125" display="https://www.metrology.net/wiki/source-time-marker/" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="C127" r:id="rId126" display="https://www.metrology.net/wiki/testprocess-source-torque/" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="C128" r:id="rId127" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="C129" r:id="rId128" display="https://www.metrology.net/wiki/testprocess-source-voltage-dc/" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="C130" r:id="rId129" display="https://www.metrology.net/wiki/source-voltage-dc-delta/" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="C131" r:id="rId130" display="https://www.metrology.net/wiki/testprocess-source-voltage-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="C132" r:id="rId131" display="https://www.metrology.net/wiki/testprocess-source-voltage-shorted/" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="C133" r:id="rId132" display="https://www.metrology.net/wiki/testprocess-source-weight/" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-conductance/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductivity/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId5" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://www.metrology.net/wiki/testprocess-measure-current-dc/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId8" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId10" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId11" display="https://www.metrology.net/wiki/testprocess-measure-force/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId12" display="https://www.metrology.net/wiki/testprocess-measure-frequency/" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId13" display="https://www.metrology.net/wiki/testprocess-measure-frequency-amplitudemodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId14" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-deviation/" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId15" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId16" display="https://www.metrology.net/wiki/testprocess-measure-frequency-phasemodulation-rate/" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId17" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId18" display="https://www.metrology.net/wiki/testprocess-measure-impedance/" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId19" display="https://www.metrology.net/wiki/testprocess-measure-inductance/" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId20" display="https://www.metrology.net/wiki/testprocess-measure-length/" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId21" display="https://www.metrology.net/wiki/testprocess-measure-length-circumference/" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId22" display="https://www.metrology.net/wiki/testprocess-measure-length-diameter/" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId23" display="https://www.metrology.net/wiki/testprocess-measure-length-form-flatness/" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId24" display="https://www.metrology.net/wiki/testprocess-measure-length-form-parallelism/" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId25" display="https://www.metrology.net/wiki/testprocess-measure-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId26" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roughness/" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId27" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId28" display="https://www.metrology.net/wiki/testprocess-measure-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId29" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-axis/" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId30" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-surface/" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId31" display="https://www.metrology.net/wiki/testprocess-measure-length-radius/" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId32" display="https://www.metrology.net/wiki/testprocess-measure-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId33" display="https://www.metrology.net/wiki/testprocess-measure-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId34" display="https://www.metrology.net/wiki/testprocess-measure-mass-true/" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId35" display="https://www.metrology.net/wiki/testprocess-measure-phase-phasemodulation/" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId36" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId37" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent/" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C40" r:id="rId38" display="https://www.metrology.net/wiki/testprocess-measure-phasenoise-sideband/" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C41" r:id="rId39" display="https://www.metrology.net/wiki/testprocess-measure-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C42" r:id="rId40" display="https://www.metrology.net/wiki/testprocess-measure-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C43" r:id="rId41" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C44" r:id="rId42" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C45" r:id="rId43" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C46" r:id="rId44" display="https://www.metrology.net/wiki/testprocess-measure-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C47" r:id="rId45" display="https://www.metrology.net/wiki/testprocess-measure-ratio-density-mass/" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C48" r:id="rId46" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C49" r:id="rId47" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C50" r:id="rId48" display="https://www.metrology.net/wiki/testprocess-measure-ratio-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C51" r:id="rId49" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C52" r:id="rId50" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-power/" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C53" r:id="rId51" display="https://www.metrology.net/wiki/testprocess-measure-ratio-transmissioncoefficent/" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C54" r:id="rId52" display="https://www.metrology.net/wiki/testprocess-measure-ratio-torque/" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C55" r:id="rId53" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-ripple-ondc/" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C56" r:id="rId54" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C57" r:id="rId55" display="https://www.metrology.net/wiki/testprocess-measure-ratio-volts-ac-sinewave-delta-volts/" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C58" r:id="rId56" display="https://www.metrology.net/wiki/testprocess-measure-ohms/" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C59" r:id="rId57" display="https://www.metrology.net/wiki/testprocess-measure-temperature/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C60" r:id="rId58" display="https://www.metrology.net/wiki/testprocess-measure-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C61" r:id="rId59" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C62" r:id="rId60" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C63" r:id="rId61" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C64" r:id="rId62" display="https://www.metrology.net/wiki/testprocess-measure-time-pulsetransition/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C65" r:id="rId63" display="https://www.metrology.net/wiki/testprocess-measure-time-absolute/" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C66" r:id="rId64" display="https://www.metrology.net/wiki/testprocess-measure-torque/" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C67" r:id="rId65" display="https://www.metrology.net/wiki/testprocess-measure-torque-hydraulicpressure/" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C68" r:id="rId66" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac/" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C69" r:id="rId67" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-noise-ondc/" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C70" r:id="rId68" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C71" r:id="rId69" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C72" r:id="rId70" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C73" r:id="rId71" display="https://www.metrology.net/wiki/testprocess-measure-voltage-dc/" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C74" r:id="rId72" display="https://www.metrology.net/wiki/testprocess-measure-weight/" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C75" r:id="rId73" display="https://www.metrology.net/wiki/testprocess-source-capacitance/" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C76" r:id="rId74" display="https://www.metrology.net/wiki/testprocess-source-conductance/" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C77" r:id="rId75" display="https://www.metrology.net/wiki/testprocess-source-conductivity/" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C78" r:id="rId76" display="https://www.metrology.net/wiki/testprocess-source-current-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C79" r:id="rId77" display="https://www.metrology.net/wiki/testprocess-source-current-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C80" r:id="rId78" display="https://www.metrology.net/wiki/testprocess-source-current-ac-triangle/" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C81" r:id="rId79" display="https://www.metrology.net/wiki/testprocess-source-current-dc/" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C82" r:id="rId80" display="https://www.metrology.net/wiki/testprocess-source-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C83" r:id="rId81" display="https://www.metrology.net/wiki/testprocess-source-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C84" r:id="rId82" display="https://www.metrology.net/wiki/testprocess-source-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C85" r:id="rId83" display="https://www.metrology.net/wiki/testprocess-source-force/" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C86" r:id="rId84" display="https://www.metrology.net/wiki/testprocess-source-frequency-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C87" r:id="rId85" display="https://www.metrology.net/wiki/testprocess-source-frequency-arbitrary-cardiograph/" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C88" r:id="rId86" display="https://www.metrology.net/wiki/testprocess-source-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C89" r:id="rId87" display="https://www.metrology.net/wiki/testprocess-source-impedance/" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C90" r:id="rId88" display="https://www.metrology.net/wiki/testprocess-source-inductance/" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C91" r:id="rId89" display="https://www.metrology.net/wiki/testprocess-source-length/" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="C92" r:id="rId90" display="https://www.metrology.net/wiki/testprocess-source-length-circumference/" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C93" r:id="rId91" display="https://www.metrology.net/wiki/testprocess-source-length-diameter/" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C94" r:id="rId92" display="https://www.metrology.net/wiki/testprocess-source-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C95" r:id="rId93" display="https://www.metrology.net/wiki/testprocess-source-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="C96" r:id="rId94" display="https://www.metrology.net/wiki/testprocess-source-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C97" r:id="rId95" display="https://www.metrology.net/wiki/testprocess-source-length-form-straightness-surrface/" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C98" r:id="rId96" display="https://www.metrology.net/wiki/testprocess-source-length-radius/" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C99" r:id="rId97" display="https://www.metrology.net/wiki/testprocess-source-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="C100" r:id="rId98" display="https://www.metrology.net/wiki/testprocess-source-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C101" r:id="rId99" display="https://www.metrology.net/wiki/testprocess-source-mass-true/" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="C102" r:id="rId100" display="https://www.metrology.net/wiki/testprocess-source-period-marker/" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C103" r:id="rId101" display="https://www.metrology.net/wiki/testprocess-source-period-squarewave/" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C104" r:id="rId102" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C105" r:id="rId103" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave-simulated/" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C106" r:id="rId104" display="https://www.metrology.net/wiki/testprocess-source-power-dc-simulated/" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="C107" r:id="rId105" display="https://www.metrology.net/wiki/testprocess-source-power-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C108" r:id="rId106" display="https://www.metrology.net/wiki/testprocess-source-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="C109" r:id="rId107" display="https://www.metrology.net/wiki/testprocess-source-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C110" r:id="rId108" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C111" r:id="rId109" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="C112" r:id="rId110" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C113" r:id="rId111" display="https://www.metrology.net/wiki/testprocess-source-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="C114" r:id="rId112" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="C115" r:id="rId113" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="C116" r:id="rId114" display="https://www.metrology.net/wiki/testprocess-source-ratio-rf-sinusoidal-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="C117" r:id="rId115" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="C118" r:id="rId116" display="https://www.metrology.net/wiki/testprocess-source-voltage-ac-sinewave-delta-voltage/" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C119" r:id="rId117" display="https://www.metrology.net/wiki/testprocess-source-resistance/" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="C120" r:id="rId118" display="https://www.metrology.net/wiki/testprocess-source-temperature/" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="C121" r:id="rId119" display="https://www.metrology.net/wiki/testprocess-source-temperature-fixedpoint/" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="C122" r:id="rId120" display="https://www.metrology.net/wiki/testprocess-source-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="C123" r:id="rId121" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="C124" r:id="rId122" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="C125" r:id="rId123" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="C126" r:id="rId124" display="https://www.metrology.net/wiki/source-time-marker/" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="C127" r:id="rId125" display="https://www.metrology.net/wiki/testprocess-source-torque/" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="C128" r:id="rId126" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="C129" r:id="rId127" display="https://www.metrology.net/wiki/testprocess-source-voltage-dc/" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="C130" r:id="rId128" display="https://www.metrology.net/wiki/source-voltage-dc-delta/" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="C131" r:id="rId129" display="https://www.metrology.net/wiki/testprocess-source-voltage-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="C132" r:id="rId130" display="https://www.metrology.net/wiki/testprocess-source-voltage-shorted/" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="C133" r:id="rId131" display="https://www.metrology.net/wiki/testprocess-source-weight/" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId133"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId132"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6D6EC4-A3DC-42B4-ABAF-F3EE7418B168}">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" ht="45">
-      <c r="A2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" t="s">
-        <v>502</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>510</v>
-      </c>
-      <c r="E2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" t="s">
-        <v>508</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2">
-        <v>9218</v>
-      </c>
-      <c r="K2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" t="s">
-        <v>503</v>
-      </c>
-      <c r="C3" t="s">
-        <v>509</v>
-      </c>
-      <c r="E3" t="s">
-        <v>506</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3">
-        <v>2970</v>
-      </c>
-      <c r="K3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" t="s">
-        <v>505</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T8"/>
@@ -5198,29 +5063,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC584196-9739-4B08-B7A7-EF0413D9DC9F}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>458</v>
@@ -5232,31 +5097,28 @@
         <v>448</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>123</v>
+        <v>444</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="K1" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B2" t="s">
         <v>443</v>
@@ -5268,30 +5130,27 @@
         <v>363</v>
       </c>
       <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
         <v>359</v>
       </c>
-      <c r="F2" t="s">
-        <v>83</v>
-      </c>
       <c r="G2" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="H2" t="s">
-        <v>364</v>
-      </c>
-      <c r="I2" t="s">
         <v>365</v>
       </c>
-      <c r="J2">
+      <c r="I2">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B3" t="s">
         <v>443</v>
@@ -5303,27 +5162,24 @@
         <v>437</v>
       </c>
       <c r="E3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F3" t="s">
         <v>438</v>
       </c>
+      <c r="G3" t="s">
+        <v>364</v>
+      </c>
       <c r="H3" t="s">
-        <v>364</v>
-      </c>
-      <c r="I3" t="s">
         <v>439</v>
       </c>
-      <c r="J3">
+      <c r="I3">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B4" t="s">
         <v>443</v>
@@ -5335,50 +5191,47 @@
         <v>451</v>
       </c>
       <c r="E4" t="s">
-        <v>359</v>
-      </c>
-      <c r="F4" t="s">
         <v>450</v>
       </c>
+      <c r="G4" t="s">
+        <v>364</v>
+      </c>
       <c r="H4" t="s">
-        <v>364</v>
+        <v>452</v>
       </c>
       <c r="I4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="J4" t="s">
-        <v>453</v>
-      </c>
-      <c r="K4" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B5" t="s">
+        <v>467</v>
+      </c>
+      <c r="C5" t="s">
         <v>468</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>469</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>471</v>
+      </c>
+      <c r="G5" t="s">
         <v>470</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
+        <v>497</v>
+      </c>
+      <c r="I5" t="s">
         <v>472</v>
       </c>
-      <c r="H5" t="s">
-        <v>471</v>
-      </c>
-      <c r="I5" t="s">
-        <v>500</v>
-      </c>
-      <c r="J5" t="s">
-        <v>473</v>
-      </c>
-      <c r="K5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -5798,6 +5651,1885 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EB6A2-D607-49A1-9D65-9E8022B0E74E}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>538</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="30">
+      <c r="A2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>461</v>
+      </c>
+      <c r="C2" t="s">
+        <v>508</v>
+      </c>
+      <c r="D2" t="s">
+        <v>509</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="F2" t="s">
+        <v>510</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D3" t="s">
+        <v>412</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>405</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="111.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>460</v>
+      </c>
+      <c r="C4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" t="s">
+        <v>496</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="F4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>404</v>
+      </c>
+      <c r="C6" t="s">
+        <v>401</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="A7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C7" t="s">
+        <v>402</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>460</v>
+      </c>
+      <c r="C8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="255">
+      <c r="A9" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>515</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>522</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>524</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>530</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>525</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45">
+      <c r="A10" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>521</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>523</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>527</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>529</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{0EF2E425-2B27-4C14-9F80-FC65046930C8}">
+      <formula1>statementCategories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G2" t="s">
+        <v>365</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D3" t="s">
+        <v>438</v>
+      </c>
+      <c r="F3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" t="s">
+        <v>439</v>
+      </c>
+      <c r="H3">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B4" t="s">
+        <v>449</v>
+      </c>
+      <c r="C4" t="s">
+        <v>451</v>
+      </c>
+      <c r="D4" t="s">
+        <v>450</v>
+      </c>
+      <c r="F4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G4" t="s">
+        <v>452</v>
+      </c>
+      <c r="H4" t="s">
+        <v>453</v>
+      </c>
+      <c r="I4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164255F3-93CF-4992-BB4A-5F2B2030CF33}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F1" t="s">
+        <v>539</v>
+      </c>
+      <c r="G1" t="s">
+        <v>540</v>
+      </c>
+      <c r="H1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B5" t="s">
+        <v>429</v>
+      </c>
+      <c r="C5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D5" t="s">
+        <v>426</v>
+      </c>
+      <c r="E5" t="s">
+        <v>425</v>
+      </c>
+      <c r="F5" t="s">
+        <v>424</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" t="s">
+        <v>427</v>
+      </c>
+      <c r="D6" t="s">
+        <v>426</v>
+      </c>
+      <c r="E6" t="s">
+        <v>425</v>
+      </c>
+      <c r="F6" t="s">
+        <v>424</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>421</v>
+      </c>
+      <c r="B7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E7" t="s">
+        <v>417</v>
+      </c>
+      <c r="F7" t="s">
+        <v>416</v>
+      </c>
+      <c r="H7">
+        <v>9.9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>421</v>
+      </c>
+      <c r="B8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C8" t="s">
+        <v>419</v>
+      </c>
+      <c r="D8" t="s">
+        <v>418</v>
+      </c>
+      <c r="E8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F8" t="s">
+        <v>416</v>
+      </c>
+      <c r="H8">
+        <v>0.99</v>
+      </c>
+      <c r="I8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B9" t="s">
+        <v>420</v>
+      </c>
+      <c r="C9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D9" t="s">
+        <v>418</v>
+      </c>
+      <c r="E9" t="s">
+        <v>417</v>
+      </c>
+      <c r="F9" t="s">
+        <v>416</v>
+      </c>
+      <c r="H9">
+        <v>9.9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>421</v>
+      </c>
+      <c r="B10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C10" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10" t="s">
+        <v>433</v>
+      </c>
+      <c r="E10" t="s">
+        <v>434</v>
+      </c>
+      <c r="F10" t="s">
+        <v>435</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D53FE5-FD05-490B-BD2B-60774A285524}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="72.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="75" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E2">
+        <v>255</v>
+      </c>
+      <c r="F2">
+        <v>17025</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="209.25" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:P40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+    </row>
+    <row r="2" spans="1:16" ht="17.25" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="26">
+        <f>COUNTA(B9:XFD9)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="23.25">
+      <c r="A10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="23.25">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="23.25">
+      <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="23.25">
+      <c r="A13" s="35" t="s">
+        <v>487</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>521</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>398</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>491</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="34.5">
+      <c r="A14" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0</v>
+      </c>
+      <c r="D15" s="18">
+        <f>ROUND(E15+273.15,2)</f>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="G15" s="9">
+        <f>ROUND(F15-E15,1)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I15" s="25">
+        <v>2</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="8">
+        <v>1</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="17">
+        <v>15</v>
+      </c>
+      <c r="D16" s="18">
+        <f t="shared" ref="D16:D19" si="0">ROUND(E16+273.15,2)</f>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" ref="G16:G19" si="1">ROUND(F16-E16,1)</f>
+        <v>15.1</v>
+      </c>
+      <c r="H16" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I16" s="25">
+        <v>2</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="8">
+        <v>2</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="17">
+        <v>25</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" si="0"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="9">
+        <v>25.2</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="1"/>
+        <v>25.2</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="25">
+        <v>2</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="8">
+        <v>3</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="17">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18">
+        <f t="shared" si="0"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="9">
+        <v>15.3</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>15.3</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I18" s="25">
+        <v>2</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="8">
+        <v>4</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0</v>
+      </c>
+      <c r="D19" s="18">
+        <f t="shared" si="0"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I19" s="25">
+        <v>2</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="4">
+        <v>5</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="26">
+        <f>COUNTA(B30:XFD30)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="23.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="23.25">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="23.25">
+      <c r="A33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="35" t="s">
+        <v>487</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="K34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="L34" s="34" t="s">
+        <v>489</v>
+      </c>
+      <c r="M34" s="34" t="s">
+        <v>521</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>398</v>
+      </c>
+      <c r="O34" s="34" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="34.5">
+      <c r="A35" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="N35" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="O35" s="22" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="17">
+        <v>0</v>
+      </c>
+      <c r="D36" s="18">
+        <f>ROUND(E36+273.15,2)</f>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E36" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="F36" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="G36" s="9">
+        <f>ROUND(F36-E36,1)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="H36" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I36" s="25">
+        <v>2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L36" s="8">
+        <v>1</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N36" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="17">
+        <v>15</v>
+      </c>
+      <c r="D37" s="18">
+        <f t="shared" ref="D37:D40" si="2">ROUND(E37+273.15,2)</f>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E37" s="18">
+        <v>15.01</v>
+      </c>
+      <c r="F37" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" ref="G37:G40" si="3">ROUND(F37-E37,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="25">
+        <v>2</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L37" s="8">
+        <v>2</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N37" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="O37" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="17">
+        <v>25</v>
+      </c>
+      <c r="D38" s="18">
+        <f t="shared" si="2"/>
+        <v>298.17</v>
+      </c>
+      <c r="E38" s="18">
+        <v>25.02</v>
+      </c>
+      <c r="F38" s="9">
+        <v>25.2</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I38" s="25">
+        <v>2</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L38" s="8">
+        <v>3</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="O38" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="17">
+        <v>15</v>
+      </c>
+      <c r="D39" s="18">
+        <f t="shared" si="2"/>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E39" s="18">
+        <v>15.01</v>
+      </c>
+      <c r="F39" s="9">
+        <v>15.3</v>
+      </c>
+      <c r="G39" s="9">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="H39" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I39" s="25">
+        <v>2</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="8">
+        <v>4</v>
+      </c>
+      <c r="M39" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="N39" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="O39" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="20">
+        <v>0</v>
+      </c>
+      <c r="D40" s="18">
+        <f t="shared" si="2"/>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E40" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+      <c r="G40" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I40" s="25">
+        <v>2</v>
+      </c>
+      <c r="J40" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40" s="4">
+        <v>5</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>492</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:P11 B32:O32" xr:uid="{00000000-0002-0000-0500-000000000000}">
+      <formula1>MeasurandType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:P9 B30:O30" xr:uid="{00000000-0002-0000-0500-000001000000}">
+      <formula1>ColType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:P10 B31:O31" xr:uid="{00000000-0002-0000-0500-000002000000}">
+      <formula1>MetaType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:P13 B34:O34" xr:uid="{FB1CB67C-7785-4D42-8012-3FA40F22C35C}">
+      <formula1>metaDataType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I1"/>
@@ -5853,1933 +7585,145 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EB6A2-D607-49A1-9D65-9E8022B0E74E}">
-  <dimension ref="A1:H8"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6D6EC4-A3DC-42B4-ABAF-F3EE7418B168}">
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="30">
-      <c r="A2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>462</v>
-      </c>
-      <c r="C2" t="s">
-        <v>511</v>
-      </c>
-      <c r="D2" t="s">
-        <v>512</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>409</v>
-      </c>
-      <c r="F2" t="s">
-        <v>513</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30">
-      <c r="A3" t="s">
-        <v>390</v>
-      </c>
-      <c r="B3" t="s">
-        <v>461</v>
-      </c>
-      <c r="C3" t="s">
-        <v>372</v>
-      </c>
-      <c r="D3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>405</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>413</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="111.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>390</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="C4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D4" t="s">
-        <v>499</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>498</v>
-      </c>
-      <c r="F4" t="s">
-        <v>499</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30">
-      <c r="A5" t="s">
-        <v>390</v>
-      </c>
-      <c r="B5" t="s">
-        <v>404</v>
-      </c>
-      <c r="C5" t="s">
-        <v>400</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30">
-      <c r="A6" t="s">
-        <v>390</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>404</v>
-      </c>
-      <c r="C6" t="s">
-        <v>401</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45">
-      <c r="A7" t="s">
-        <v>390</v>
-      </c>
-      <c r="B7" t="s">
-        <v>404</v>
-      </c>
-      <c r="C7" t="s">
-        <v>402</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>390</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="C8" t="s">
-        <v>495</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{0EF2E425-2B27-4C14-9F80-FC65046930C8}">
-      <formula1>statementCategories</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>448</v>
+        <v>480</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>121</v>
+        <v>481</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>122</v>
+        <v>504</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>123</v>
+        <v>478</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>445</v>
+        <v>479</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>446</v>
+        <v>482</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11">
+        <v>483</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="45">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C2" t="s">
-        <v>363</v>
-      </c>
-      <c r="D2" t="s">
-        <v>359</v>
+        <v>499</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>507</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G2" t="s">
-        <v>364</v>
+        <v>505</v>
       </c>
       <c r="H2" t="s">
-        <v>365</v>
+        <v>109</v>
       </c>
       <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>9218</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>443</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>436</v>
+        <v>500</v>
       </c>
       <c r="C3" t="s">
-        <v>437</v>
-      </c>
-      <c r="D3" t="s">
-        <v>359</v>
+        <v>506</v>
       </c>
       <c r="E3" t="s">
-        <v>438</v>
-      </c>
-      <c r="G3" t="s">
-        <v>364</v>
+        <v>503</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>439</v>
+        <v>92</v>
       </c>
       <c r="I3">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>2970</v>
+      </c>
+      <c r="K3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>443</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>449</v>
-      </c>
-      <c r="C4" t="s">
-        <v>451</v>
-      </c>
-      <c r="D4" t="s">
-        <v>359</v>
-      </c>
-      <c r="E4" t="s">
-        <v>450</v>
-      </c>
-      <c r="G4" t="s">
-        <v>364</v>
-      </c>
-      <c r="H4" t="s">
-        <v>452</v>
-      </c>
-      <c r="I4" t="s">
-        <v>453</v>
-      </c>
-      <c r="J4" t="s">
-        <v>454</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>502</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164255F3-93CF-4992-BB4A-5F2B2030CF33}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="55.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F1" t="s">
-        <v>410</v>
-      </c>
-      <c r="G1" t="s">
-        <v>430</v>
-      </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B5" t="s">
-        <v>429</v>
-      </c>
-      <c r="C5" t="s">
-        <v>427</v>
-      </c>
-      <c r="D5" t="s">
-        <v>426</v>
-      </c>
-      <c r="E5" t="s">
-        <v>425</v>
-      </c>
-      <c r="F5" t="s">
-        <v>424</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>421</v>
-      </c>
-      <c r="B6" t="s">
-        <v>428</v>
-      </c>
-      <c r="C6" t="s">
-        <v>427</v>
-      </c>
-      <c r="D6" t="s">
-        <v>426</v>
-      </c>
-      <c r="E6" t="s">
-        <v>425</v>
-      </c>
-      <c r="F6" t="s">
-        <v>424</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>421</v>
-      </c>
-      <c r="B7" t="s">
-        <v>423</v>
-      </c>
-      <c r="C7" t="s">
-        <v>419</v>
-      </c>
-      <c r="D7" t="s">
-        <v>418</v>
-      </c>
-      <c r="E7" t="s">
-        <v>417</v>
-      </c>
-      <c r="F7" t="s">
-        <v>416</v>
-      </c>
-      <c r="G7">
-        <v>9.9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>421</v>
-      </c>
-      <c r="B8" t="s">
-        <v>422</v>
-      </c>
-      <c r="C8" t="s">
-        <v>419</v>
-      </c>
-      <c r="D8" t="s">
-        <v>418</v>
-      </c>
-      <c r="E8" t="s">
-        <v>417</v>
-      </c>
-      <c r="F8" t="s">
-        <v>416</v>
-      </c>
-      <c r="G8">
-        <v>0.99</v>
-      </c>
-      <c r="H8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>421</v>
-      </c>
-      <c r="B9" t="s">
-        <v>420</v>
-      </c>
-      <c r="C9" t="s">
-        <v>419</v>
-      </c>
-      <c r="D9" t="s">
-        <v>418</v>
-      </c>
-      <c r="E9" t="s">
-        <v>417</v>
-      </c>
-      <c r="F9" t="s">
-        <v>416</v>
-      </c>
-      <c r="G9">
-        <v>9.9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>421</v>
-      </c>
-      <c r="B10" t="s">
-        <v>431</v>
-      </c>
-      <c r="C10" t="s">
-        <v>432</v>
-      </c>
-      <c r="D10" t="s">
-        <v>433</v>
-      </c>
-      <c r="E10" t="s">
-        <v>434</v>
-      </c>
-      <c r="F10" t="s">
-        <v>435</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D53FE5-FD05-490B-BD2B-60774A285524}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="72.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
-    <col min="8" max="8" width="75" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>518</v>
-      </c>
-      <c r="B2" t="s">
-        <v>535</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E2">
-        <v>255</v>
-      </c>
-      <c r="F2">
-        <v>17025</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="209.25" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE2214C-3734-4A04-94FA-9C722A83E994}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="57.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="61.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="270" customHeight="1">
-      <c r="A2" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>461</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>525</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>527</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>533</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>528</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="65.25" customHeight="1">
-      <c r="A3" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>404</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>526</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>529</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>531</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>530</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>532</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{0DE352B7-7F5B-4D6F-B654-B1F6857FA0A4}">
-      <formula1>statementCategories</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:P40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>441</v>
-      </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-    </row>
-    <row r="2" spans="1:16" ht="17.25" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="26">
-        <f>COUNTA(B9:XFD9)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="23.25">
-      <c r="A10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="23.25">
-      <c r="A11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="23.25">
-      <c r="A12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>491</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="O12" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="P12" s="14" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="23.25">
-      <c r="A13" s="35" t="s">
-        <v>488</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="L13" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="M13" s="34" t="s">
-        <v>524</v>
-      </c>
-      <c r="N13" s="34" t="s">
-        <v>398</v>
-      </c>
-      <c r="O13" s="34" t="s">
-        <v>493</v>
-      </c>
-      <c r="P13" s="34" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="34.5">
-      <c r="A14" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="N14" s="22" t="s">
-        <v>399</v>
-      </c>
-      <c r="O14" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="P14" s="22" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="17">
-        <v>0</v>
-      </c>
-      <c r="D15" s="18">
-        <f>ROUND(E15+273.15,2)</f>
-        <v>273.14999999999998</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="9">
-        <v>-0.1</v>
-      </c>
-      <c r="G15" s="9">
-        <f>ROUND(F15-E15,1)</f>
-        <v>-0.1</v>
-      </c>
-      <c r="H15" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I15" s="25">
-        <v>2</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="8">
-        <v>1</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="17">
-        <v>15</v>
-      </c>
-      <c r="D16" s="18">
-        <f t="shared" ref="D16:D19" si="0">ROUND(E16+273.15,2)</f>
-        <v>273.14999999999998</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" ref="G16:G19" si="1">ROUND(F16-E16,1)</f>
-        <v>15.1</v>
-      </c>
-      <c r="H16" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I16" s="25">
-        <v>2</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" s="8">
-        <v>2</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="P16" s="9" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="17">
-        <v>25</v>
-      </c>
-      <c r="D17" s="18">
-        <f t="shared" si="0"/>
-        <v>273.14999999999998</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="9">
-        <v>25.2</v>
-      </c>
-      <c r="G17" s="9">
-        <f t="shared" si="1"/>
-        <v>25.2</v>
-      </c>
-      <c r="H17" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I17" s="25">
-        <v>2</v>
-      </c>
-      <c r="J17" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" s="8">
-        <v>3</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="17">
-        <v>15</v>
-      </c>
-      <c r="D18" s="18">
-        <f t="shared" si="0"/>
-        <v>273.14999999999998</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="9">
-        <v>15.3</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="1"/>
-        <v>15.3</v>
-      </c>
-      <c r="H18" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I18" s="25">
-        <v>2</v>
-      </c>
-      <c r="J18" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="8">
-        <v>4</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="20">
-        <v>0</v>
-      </c>
-      <c r="D19" s="18">
-        <f t="shared" si="0"/>
-        <v>273.14999999999998</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I19" s="25">
-        <v>2</v>
-      </c>
-      <c r="J19" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L19" s="4">
-        <v>5</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="P19" s="9" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="26">
-        <f>COUNTA(B30:XFD30)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="N30" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="O30" s="11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="23.25">
-      <c r="A31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="N31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O31" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="23.25">
-      <c r="A32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="M32" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="N32" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="O32" s="11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="23.25">
-      <c r="A33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>491</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M33" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="N33" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="O33" s="14" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="35" t="s">
-        <v>488</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="J34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="K34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="L34" s="34" t="s">
-        <v>490</v>
-      </c>
-      <c r="M34" s="34" t="s">
-        <v>524</v>
-      </c>
-      <c r="N34" s="34" t="s">
-        <v>398</v>
-      </c>
-      <c r="O34" s="34" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="34.5">
-      <c r="A35" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K35" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="L35" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="N35" s="22" t="s">
-        <v>399</v>
-      </c>
-      <c r="O35" s="22" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="17">
-        <v>0</v>
-      </c>
-      <c r="D36" s="18">
-        <f>ROUND(E36+273.15,2)</f>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E36" s="18">
-        <v>0.01</v>
-      </c>
-      <c r="F36" s="9">
-        <v>-0.1</v>
-      </c>
-      <c r="G36" s="9">
-        <f>ROUND(F36-E36,1)</f>
-        <v>-0.1</v>
-      </c>
-      <c r="H36" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I36" s="25">
-        <v>2</v>
-      </c>
-      <c r="J36" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L36" s="8">
-        <v>1</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="17">
-        <v>15</v>
-      </c>
-      <c r="D37" s="18">
-        <f t="shared" ref="D37:D40" si="2">ROUND(E37+273.15,2)</f>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E37" s="18">
-        <v>15.01</v>
-      </c>
-      <c r="F37" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G37" s="9">
-        <f t="shared" ref="G37:G40" si="3">ROUND(F37-E37,1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H37" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I37" s="25">
-        <v>2</v>
-      </c>
-      <c r="J37" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L37" s="8">
-        <v>2</v>
-      </c>
-      <c r="M37" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N37" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="O37" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="17">
-        <v>25</v>
-      </c>
-      <c r="D38" s="18">
-        <f t="shared" si="2"/>
-        <v>298.17</v>
-      </c>
-      <c r="E38" s="18">
-        <v>25.02</v>
-      </c>
-      <c r="F38" s="9">
-        <v>25.2</v>
-      </c>
-      <c r="G38" s="9">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="H38" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I38" s="25">
-        <v>2</v>
-      </c>
-      <c r="J38" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L38" s="8">
-        <v>3</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="17">
-        <v>15</v>
-      </c>
-      <c r="D39" s="18">
-        <f t="shared" si="2"/>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E39" s="18">
-        <v>15.01</v>
-      </c>
-      <c r="F39" s="9">
-        <v>15.3</v>
-      </c>
-      <c r="G39" s="9">
-        <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="H39" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I39" s="25">
-        <v>2</v>
-      </c>
-      <c r="J39" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L39" s="8">
-        <v>4</v>
-      </c>
-      <c r="M39" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="N39" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="20">
-        <v>0</v>
-      </c>
-      <c r="D40" s="18">
-        <f t="shared" si="2"/>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E40" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="F40" s="7">
-        <v>0</v>
-      </c>
-      <c r="G40" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I40" s="25">
-        <v>2</v>
-      </c>
-      <c r="J40" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L40" s="4">
-        <v>5</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="O40" s="7" t="s">
-        <v>494</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <mergeCells count="1">
-    <mergeCell ref="G1:K1"/>
-  </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:P11 B32:O32" xr:uid="{00000000-0002-0000-0500-000000000000}">
-      <formula1>MeasurandType</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:P9 B30:O30" xr:uid="{00000000-0002-0000-0500-000001000000}">
-      <formula1>ColType</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:P10 B31:O31" xr:uid="{00000000-0002-0000-0500-000002000000}">
-      <formula1>MetaType</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:P13 B34:O34" xr:uid="{FB1CB67C-7785-4D42-8012-3FA40F22C35C}">
-      <formula1>metaDataType</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>